<commit_message>
Update homework-01-final-grade.xlsx with comment
</commit_message>
<xml_diff>
--- a/Supplements/homework-01-final-grade.xlsx
+++ b/Supplements/homework-01-final-grade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/研究生课程/多核程序设计与实践（助教）/homework-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7851D9-9150-6A42-B4AF-66D10AD6669D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F7B323-8EAB-214F-9B0A-0BC7F7E5063A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,17 @@
     <sheet name="Sheet 1 - res" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1 - res'!$L$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1 - res'!$L$2:$L$134</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1 - res'!$F$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1 - res'!$F$3:$F$113</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1 - res'!$F$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1 - res'!$F$3:$F$118</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1 - res'!$L$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1 - res'!$L$2:$L$139</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="182">
   <si>
     <t>实验报告</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -970,6 +970,48 @@
   <si>
     <t>程序运行出现段错误</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>提交的作业命名有问题，需要手动修改名称后才能正常运行</t>
+  </si>
+  <si>
+    <t>编译失败，提交的源代码字符编码错误</t>
+  </si>
+  <si>
+    <t>OpenMP源代码编译失败</t>
+  </si>
+  <si>
+    <t>c851e3401288ec3ef85dd716110f9bf5</t>
+  </si>
+  <si>
+    <t>e1a955c91078bc8ca96bc549df907c4a</t>
+  </si>
+  <si>
+    <t>3a8f0d172c9f9835df0987a1ce98b2c7</t>
+  </si>
+  <si>
+    <t>460d570838553f63cef493df91113433</t>
+  </si>
+  <si>
+    <t>0f3cdcf7250a6e41949b8be3afeb7719</t>
+  </si>
+  <si>
+    <t>c94f554a2121ee7fb239f1fadcc398f3</t>
   </si>
 </sst>
 </file>
@@ -1141,7 +1183,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1298,6 +1340,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1407,7 +1452,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1499,7 +1544,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{1030102B-0947-CA47-9ED9-857AE3CBF761}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>时间（ms）</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1528,7 +1573,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1574,7 +1619,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{782EC41C-AD7D-E542-8EB7-0E8059F39A56}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>总分</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3925,10 +3970,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:II134"/>
+  <dimension ref="A1:II139"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="25" customHeight="1"/>
@@ -3955,22 +4000,22 @@
       <c r="A1" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="54" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="52" t="s">
+      <c r="B1" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="55"/>
+      <c r="D1" s="55"/>
+      <c r="E1" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="53" t="s">
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
       <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
@@ -4078,7 +4123,7 @@
         <v>136.96</v>
       </c>
       <c r="G4" s="39">
-        <f t="shared" ref="G4:G72" si="1">IF(F4&gt;0, IF(F4&lt;2, 30, IF(F4&gt;100, 10, (1-(F4-2)/(100-2))*20+10)), 0)</f>
+        <f t="shared" ref="G4:G77" si="1">IF(F4&gt;0, IF(F4&lt;2, 30, IF(F4&gt;100, 10, (1-(F4-2)/(100-2))*20+10)), 0)</f>
         <v>10</v>
       </c>
       <c r="H4" s="33">
@@ -5163,7 +5208,7 @@
         <v>5</v>
       </c>
       <c r="I30" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J30" s="2">
         <v>0</v>
@@ -5175,9 +5220,7 @@
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="M30" s="26" t="s">
-        <v>153</v>
-      </c>
+      <c r="M30" s="26"/>
     </row>
     <row r="31" spans="1:13" ht="25" customHeight="1">
       <c r="A31" s="11" t="s">
@@ -6928,7 +6971,7 @@
         <v>5</v>
       </c>
       <c r="L50" s="3">
-        <f t="shared" ref="L50:L83" si="2">IF(SUM(B50:E50,G50,H50:I50,K50)&lt;100, SUM(B50:E50,G50,H50:I50,K50),  100)</f>
+        <f t="shared" ref="L50:L88" si="2">IF(SUM(B50:E50,G50,H50:I50,K50)&lt;100, SUM(B50:E50,G50,H50:I50,K50),  100)</f>
         <v>70</v>
       </c>
       <c r="M50" s="26" t="s">
@@ -6977,215 +7020,222 @@
       <c r="M51" s="27"/>
     </row>
     <row r="52" spans="1:243" ht="25" customHeight="1">
-      <c r="A52" s="24" t="s">
-        <v>25</v>
+      <c r="A52" s="11" t="s">
+        <v>63</v>
       </c>
       <c r="B52" s="16">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C52" s="16">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D52" s="1">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E52" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F52" s="35">
-        <v>1.167</v>
+        <v>0</v>
       </c>
       <c r="G52" s="39">
-        <f>IF(F52&gt;0, IF(F52&lt;2, 30, IF(F52&gt;100, 10, (1-(F52-2)/(100-2))*20+10)), 0)</f>
-        <v>30</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H52" s="33">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I52" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J52" s="2">
         <v>0</v>
       </c>
       <c r="K52" s="4">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L52" s="3">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="M52" s="26"/>
+        <v>20</v>
+      </c>
+      <c r="M52" s="27" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="53" spans="1:243" ht="25" customHeight="1">
       <c r="A53" s="11" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B53" s="16">
+        <v>10</v>
+      </c>
+      <c r="C53" s="19">
+        <v>10</v>
+      </c>
+      <c r="D53" s="1">
         <v>8</v>
       </c>
-      <c r="C53" s="16">
-        <v>3</v>
-      </c>
-      <c r="D53" s="1">
-        <v>3</v>
-      </c>
       <c r="E53" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F53" s="35">
-        <v>0</v>
+        <v>14.272</v>
       </c>
       <c r="G53" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>27.495510204081633</v>
       </c>
       <c r="H53" s="33">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I53" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J53" s="2">
-        <v>0</v>
+        <v>0.48080000000000001</v>
       </c>
       <c r="K53" s="4">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L53" s="3">
         <f t="shared" si="2"/>
-        <v>20</v>
-      </c>
-      <c r="M53" s="27" t="s">
-        <v>161</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M53" s="26"/>
+      <c r="IG53" s="7"/>
+      <c r="IH53" s="7"/>
+      <c r="II53" s="7"/>
     </row>
     <row r="54" spans="1:243" ht="25" customHeight="1">
-      <c r="A54" s="11" t="s">
-        <v>64</v>
+      <c r="A54" s="52" t="s">
+        <v>176</v>
       </c>
       <c r="B54" s="16">
-        <v>10</v>
-      </c>
-      <c r="C54" s="19">
-        <v>10</v>
-      </c>
-      <c r="D54" s="1">
         <v>8</v>
       </c>
+      <c r="C54" s="16">
+        <v>7</v>
+      </c>
+      <c r="D54" s="16" t="s">
+        <v>168</v>
+      </c>
       <c r="E54" s="33">
         <v>30</v>
       </c>
       <c r="F54" s="35">
-        <v>14.272</v>
+        <v>95.793999999999997</v>
       </c>
       <c r="G54" s="39">
         <f t="shared" si="1"/>
-        <v>27.495510204081633</v>
+        <v>10.858367346938776</v>
       </c>
       <c r="H54" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I54" s="33">
         <v>10</v>
       </c>
       <c r="J54" s="2">
-        <v>0.48080000000000001</v>
+        <v>0</v>
       </c>
       <c r="K54" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L54" s="3">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="M54" s="26"/>
+        <v>73.858367346938778</v>
+      </c>
+      <c r="M54" s="26" t="s">
+        <v>173</v>
+      </c>
       <c r="IG54" s="7"/>
       <c r="IH54" s="7"/>
       <c r="II54" s="7"/>
     </row>
     <row r="55" spans="1:243" ht="25" customHeight="1">
-      <c r="A55" s="11" t="s">
-        <v>65</v>
+      <c r="A55" s="52" t="s">
+        <v>177</v>
       </c>
       <c r="B55" s="16">
-        <v>8</v>
-      </c>
-      <c r="C55" s="20">
-        <v>8</v>
-      </c>
-      <c r="D55" s="1">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C55" s="16">
+        <v>10</v>
+      </c>
+      <c r="D55" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="E55" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F55" s="35">
-        <v>110.16</v>
+        <v>0</v>
       </c>
       <c r="G55" s="39">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H55" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="I55" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J55" s="2">
-        <v>0.72140000000000004</v>
+        <v>0</v>
       </c>
       <c r="K55" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L55" s="3">
         <f t="shared" si="2"/>
-        <v>81</v>
-      </c>
-      <c r="M55" s="27"/>
+        <v>27.5</v>
+      </c>
+      <c r="M55" s="26" t="s">
+        <v>174</v>
+      </c>
       <c r="IG55" s="7"/>
       <c r="IH55" s="7"/>
       <c r="II55" s="7"/>
     </row>
     <row r="56" spans="1:243" ht="25" customHeight="1">
-      <c r="A56" s="11" t="s">
-        <v>66</v>
+      <c r="A56" s="52" t="s">
+        <v>178</v>
       </c>
       <c r="B56" s="16">
-        <v>5</v>
-      </c>
-      <c r="C56" s="19">
-        <v>5</v>
-      </c>
-      <c r="D56" s="1">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="C56" s="16">
+        <v>7</v>
+      </c>
+      <c r="D56" s="16" t="s">
+        <v>170</v>
       </c>
       <c r="E56" s="33">
         <v>30</v>
       </c>
       <c r="F56" s="35">
-        <v>1.0031000000000001</v>
+        <v>5.0987999999999998</v>
       </c>
       <c r="G56" s="39">
         <f t="shared" si="1"/>
-        <v>30</v>
+        <v>29.367591836734693</v>
       </c>
       <c r="H56" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="I56" s="33">
         <v>10</v>
       </c>
       <c r="J56" s="2">
-        <v>6.8999999999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="K56" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="L56" s="3">
         <f t="shared" si="2"/>
-        <v>93</v>
+        <v>91.36759183673469</v>
       </c>
       <c r="M56" s="26"/>
       <c r="IG56" s="7"/>
@@ -7193,150 +7243,148 @@
       <c r="II56" s="7"/>
     </row>
     <row r="57" spans="1:243" ht="25" customHeight="1">
-      <c r="A57" s="11" t="s">
-        <v>67</v>
+      <c r="A57" s="52" t="s">
+        <v>179</v>
       </c>
       <c r="B57" s="16">
-        <v>10</v>
-      </c>
-      <c r="C57" s="19">
-        <v>10</v>
-      </c>
-      <c r="D57" s="1">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="C57" s="16">
+        <v>8</v>
+      </c>
+      <c r="D57" s="16" t="s">
+        <v>171</v>
       </c>
       <c r="E57" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F57" s="35">
-        <v>0</v>
+        <v>0.29863000000000001</v>
       </c>
       <c r="G57" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H57" s="33">
         <v>5</v>
       </c>
       <c r="I57" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J57" s="2">
         <v>0</v>
       </c>
       <c r="K57" s="4">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="L57" s="3">
         <f t="shared" si="2"/>
-        <v>40</v>
-      </c>
-      <c r="M57" s="27" t="s">
-        <v>162</v>
-      </c>
+        <v>96.5</v>
+      </c>
+      <c r="M57" s="26"/>
       <c r="IG57" s="7"/>
       <c r="IH57" s="7"/>
       <c r="II57" s="7"/>
     </row>
     <row r="58" spans="1:243" ht="25" customHeight="1">
-      <c r="A58" s="11" t="s">
-        <v>68</v>
+      <c r="A58" s="52" t="s">
+        <v>180</v>
       </c>
       <c r="B58" s="16">
-        <v>8</v>
-      </c>
-      <c r="C58" s="19">
-        <v>0</v>
-      </c>
-      <c r="D58" s="1">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="C58" s="16">
+        <v>9</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>172</v>
       </c>
       <c r="E58" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F58" s="35">
-        <v>0</v>
+        <v>3.1065</v>
       </c>
       <c r="G58" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>29.774183673469388</v>
       </c>
       <c r="H58" s="33">
         <v>5</v>
       </c>
       <c r="I58" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J58" s="2">
         <v>0</v>
       </c>
       <c r="K58" s="4">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L58" s="3">
         <f t="shared" si="2"/>
-        <v>17</v>
-      </c>
-      <c r="M58" s="34" t="s">
-        <v>163</v>
-      </c>
+        <v>98.774183673469395</v>
+      </c>
+      <c r="M58" s="26"/>
       <c r="IG58" s="7"/>
       <c r="IH58" s="7"/>
       <c r="II58" s="7"/>
     </row>
     <row r="59" spans="1:243" ht="25" customHeight="1">
-      <c r="A59" s="18" t="s">
-        <v>126</v>
-      </c>
-      <c r="B59" s="18">
-        <v>9</v>
-      </c>
-      <c r="C59" s="18">
-        <v>9</v>
-      </c>
-      <c r="D59" s="18">
+      <c r="A59" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="B59" s="16">
         <v>8</v>
       </c>
-      <c r="E59" s="38">
+      <c r="C59" s="16">
+        <v>8</v>
+      </c>
+      <c r="D59" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E59" s="33">
         <v>30</v>
       </c>
       <c r="F59" s="35">
-        <v>0.92820000000000003</v>
+        <v>15.476000000000001</v>
       </c>
       <c r="G59" s="39">
         <f t="shared" si="1"/>
-        <v>30</v>
-      </c>
-      <c r="H59" s="38">
+        <v>27.249795918367347</v>
+      </c>
+      <c r="H59" s="33">
         <v>4.5</v>
       </c>
-      <c r="I59" s="38">
-        <v>10</v>
-      </c>
-      <c r="J59" s="15">
-        <v>0</v>
-      </c>
-      <c r="K59" s="18">
+      <c r="I59" s="33">
+        <v>0</v>
+      </c>
+      <c r="J59" s="2">
+        <v>0</v>
+      </c>
+      <c r="K59" s="4">
         <v>4.5</v>
       </c>
       <c r="L59" s="3">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="M59" s="27"/>
+        <v>82.24979591836734</v>
+      </c>
+      <c r="M59" s="26" t="s">
+        <v>175</v>
+      </c>
       <c r="IG59" s="7"/>
       <c r="IH59" s="7"/>
       <c r="II59" s="7"/>
     </row>
     <row r="60" spans="1:243" ht="25" customHeight="1">
       <c r="A60" s="11" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B60" s="16">
         <v>8</v>
       </c>
-      <c r="C60" s="16">
-        <v>5</v>
+      <c r="C60" s="20">
+        <v>8</v>
       </c>
       <c r="D60" s="1">
         <v>5</v>
@@ -7345,11 +7393,11 @@
         <v>30</v>
       </c>
       <c r="F60" s="35">
-        <v>79.941000000000003</v>
+        <v>110.16</v>
       </c>
       <c r="G60" s="39">
         <f t="shared" si="1"/>
-        <v>14.093673469387756</v>
+        <v>10</v>
       </c>
       <c r="H60" s="33">
         <v>5</v>
@@ -7358,42 +7406,42 @@
         <v>10</v>
       </c>
       <c r="J60" s="2">
-        <v>8.0999999999999996E-3</v>
+        <v>0.72140000000000004</v>
       </c>
       <c r="K60" s="4">
         <v>5</v>
       </c>
       <c r="L60" s="3">
         <f t="shared" si="2"/>
-        <v>82.093673469387753</v>
-      </c>
-      <c r="M60" s="26"/>
+        <v>81</v>
+      </c>
+      <c r="M60" s="27"/>
       <c r="IG60" s="7"/>
       <c r="IH60" s="7"/>
       <c r="II60" s="7"/>
     </row>
     <row r="61" spans="1:243" ht="25" customHeight="1">
       <c r="A61" s="11" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B61" s="16">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C61" s="19">
         <v>5</v>
       </c>
       <c r="D61" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E61" s="33">
         <v>30</v>
       </c>
       <c r="F61" s="35">
-        <v>0</v>
+        <v>1.0031000000000001</v>
       </c>
       <c r="G61" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H61" s="33">
         <v>5</v>
@@ -7402,164 +7450,178 @@
         <v>10</v>
       </c>
       <c r="J61" s="2">
-        <v>1.0281439999999999</v>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="K61" s="4">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="L61" s="3">
         <f t="shared" si="2"/>
-        <v>67.5</v>
-      </c>
-      <c r="M61" s="27" t="s">
-        <v>164</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="M61" s="26"/>
       <c r="IG61" s="7"/>
       <c r="IH61" s="7"/>
       <c r="II61" s="7"/>
     </row>
     <row r="62" spans="1:243" ht="25" customHeight="1">
-      <c r="A62" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="21">
-        <v>7</v>
-      </c>
-      <c r="C62" s="21">
-        <v>5</v>
-      </c>
-      <c r="D62" s="21">
-        <v>5</v>
-      </c>
-      <c r="E62" s="38">
-        <v>30</v>
+      <c r="A62" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B62" s="16">
+        <v>10</v>
+      </c>
+      <c r="C62" s="19">
+        <v>10</v>
+      </c>
+      <c r="D62" s="1">
+        <v>10</v>
+      </c>
+      <c r="E62" s="33">
+        <v>0</v>
       </c>
       <c r="F62" s="35">
-        <v>5.9455999999999998</v>
+        <v>0</v>
       </c>
       <c r="G62" s="39">
         <f t="shared" si="1"/>
-        <v>29.194775510204082</v>
-      </c>
-      <c r="H62" s="38">
-        <v>5</v>
-      </c>
-      <c r="I62" s="38">
-        <v>10</v>
-      </c>
-      <c r="J62" s="15">
-        <v>0</v>
-      </c>
-      <c r="K62" s="21">
+        <v>0</v>
+      </c>
+      <c r="H62" s="33">
+        <v>5</v>
+      </c>
+      <c r="I62" s="33">
+        <v>0</v>
+      </c>
+      <c r="J62" s="2">
+        <v>0</v>
+      </c>
+      <c r="K62" s="4">
         <v>5</v>
       </c>
       <c r="L62" s="3">
         <f t="shared" si="2"/>
-        <v>96.194775510204082</v>
-      </c>
-      <c r="M62" s="26"/>
+        <v>40</v>
+      </c>
+      <c r="M62" s="27" t="s">
+        <v>162</v>
+      </c>
       <c r="IG62" s="7"/>
       <c r="IH62" s="7"/>
       <c r="II62" s="7"/>
     </row>
     <row r="63" spans="1:243" ht="25" customHeight="1">
       <c r="A63" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B63" s="55">
-        <v>27</v>
-      </c>
-      <c r="C63" s="56"/>
-      <c r="D63" s="57"/>
+        <v>68</v>
+      </c>
+      <c r="B63" s="16">
+        <v>8</v>
+      </c>
+      <c r="C63" s="19">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
       <c r="E63" s="33">
-        <v>30</v>
-      </c>
-      <c r="F63" s="40">
-        <v>83.125</v>
+        <v>0</v>
+      </c>
+      <c r="F63" s="35">
+        <v>0</v>
       </c>
       <c r="G63" s="39">
         <f t="shared" si="1"/>
-        <v>13.443877551020408</v>
+        <v>0</v>
       </c>
       <c r="H63" s="33">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="I63" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J63" s="2">
-        <v>0.16397200000000001</v>
+        <v>0</v>
       </c>
       <c r="K63" s="4">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="L63" s="3">
         <f t="shared" si="2"/>
-        <v>89.443877551020407</v>
-      </c>
-      <c r="M63" s="27"/>
+        <v>17</v>
+      </c>
+      <c r="M63" s="34" t="s">
+        <v>163</v>
+      </c>
       <c r="IG63" s="7"/>
       <c r="IH63" s="7"/>
       <c r="II63" s="7"/>
     </row>
     <row r="64" spans="1:243" ht="25" customHeight="1">
-      <c r="A64" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64" s="55">
-        <v>30</v>
-      </c>
-      <c r="C64" s="56"/>
-      <c r="D64" s="57"/>
-      <c r="E64" s="33">
-        <v>30</v>
-      </c>
-      <c r="F64" s="40">
-        <v>86.150999999999996</v>
+      <c r="A64" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="18">
+        <v>9</v>
+      </c>
+      <c r="C64" s="18">
+        <v>9</v>
+      </c>
+      <c r="D64" s="18">
+        <v>8</v>
+      </c>
+      <c r="E64" s="38">
+        <v>30</v>
+      </c>
+      <c r="F64" s="35">
+        <v>0.92820000000000003</v>
       </c>
       <c r="G64" s="39">
         <f t="shared" si="1"/>
-        <v>12.826326530612246</v>
-      </c>
-      <c r="H64" s="33">
-        <v>5</v>
-      </c>
-      <c r="I64" s="33">
-        <v>10</v>
-      </c>
-      <c r="J64" s="2">
-        <v>0.79987600000000003</v>
-      </c>
-      <c r="K64" s="4">
-        <v>2.5</v>
+        <v>30</v>
+      </c>
+      <c r="H64" s="38">
+        <v>4.5</v>
+      </c>
+      <c r="I64" s="38">
+        <v>10</v>
+      </c>
+      <c r="J64" s="15">
+        <v>0</v>
+      </c>
+      <c r="K64" s="18">
+        <v>4.5</v>
       </c>
       <c r="L64" s="3">
         <f t="shared" si="2"/>
-        <v>90.326326530612249</v>
-      </c>
-      <c r="M64" s="26"/>
+        <v>100</v>
+      </c>
+      <c r="M64" s="27"/>
       <c r="IG64" s="7"/>
       <c r="IH64" s="7"/>
       <c r="II64" s="7"/>
     </row>
     <row r="65" spans="1:243" ht="25" customHeight="1">
       <c r="A65" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="55">
-        <v>30</v>
-      </c>
-      <c r="C65" s="56"/>
-      <c r="D65" s="57"/>
+        <v>69</v>
+      </c>
+      <c r="B65" s="16">
+        <v>8</v>
+      </c>
+      <c r="C65" s="16">
+        <v>5</v>
+      </c>
+      <c r="D65" s="1">
+        <v>5</v>
+      </c>
       <c r="E65" s="33">
         <v>30</v>
       </c>
-      <c r="F65" s="40">
-        <v>11.093</v>
+      <c r="F65" s="35">
+        <v>79.941000000000003</v>
       </c>
       <c r="G65" s="39">
         <f t="shared" si="1"/>
-        <v>28.144285714285715</v>
+        <v>14.093673469387756</v>
       </c>
       <c r="H65" s="33">
         <v>5</v>
@@ -7568,227 +7630,227 @@
         <v>10</v>
       </c>
       <c r="J65" s="2">
-        <v>5.2023E-2</v>
+        <v>8.0999999999999996E-3</v>
       </c>
       <c r="K65" s="4">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="L65" s="3">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="M65" s="25" t="s">
-        <v>133</v>
-      </c>
+        <v>82.093673469387753</v>
+      </c>
+      <c r="M65" s="26"/>
       <c r="IG65" s="7"/>
       <c r="IH65" s="7"/>
       <c r="II65" s="7"/>
     </row>
     <row r="66" spans="1:243" ht="25" customHeight="1">
       <c r="A66" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="B66" s="55">
-        <v>24</v>
-      </c>
-      <c r="C66" s="56"/>
-      <c r="D66" s="57"/>
+        <v>70</v>
+      </c>
+      <c r="B66" s="16">
+        <v>8</v>
+      </c>
+      <c r="C66" s="19">
+        <v>5</v>
+      </c>
+      <c r="D66" s="1">
+        <v>5</v>
+      </c>
       <c r="E66" s="33">
         <v>30</v>
       </c>
-      <c r="F66" s="40">
-        <v>157.71</v>
+      <c r="F66" s="35">
+        <v>0</v>
       </c>
       <c r="G66" s="39">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H66" s="33">
         <v>5</v>
       </c>
       <c r="I66" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J66" s="2">
-        <v>0</v>
+        <v>1.0281439999999999</v>
       </c>
       <c r="K66" s="4">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L66" s="3">
         <f t="shared" si="2"/>
-        <v>71.5</v>
-      </c>
-      <c r="M66" s="26" t="s">
-        <v>134</v>
+        <v>67.5</v>
+      </c>
+      <c r="M66" s="27" t="s">
+        <v>164</v>
       </c>
       <c r="IG66" s="7"/>
       <c r="IH66" s="7"/>
       <c r="II66" s="7"/>
     </row>
     <row r="67" spans="1:243" ht="25" customHeight="1">
-      <c r="A67" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="B67" s="55">
-        <v>24</v>
-      </c>
-      <c r="C67" s="56"/>
-      <c r="D67" s="57"/>
-      <c r="E67" s="33">
-        <v>0</v>
-      </c>
-      <c r="F67" s="40">
-        <v>0</v>
+      <c r="A67" s="21" t="s">
+        <v>127</v>
+      </c>
+      <c r="B67" s="21">
+        <v>7</v>
+      </c>
+      <c r="C67" s="21">
+        <v>5</v>
+      </c>
+      <c r="D67" s="21">
+        <v>5</v>
+      </c>
+      <c r="E67" s="38">
+        <v>30</v>
+      </c>
+      <c r="F67" s="35">
+        <v>5.9455999999999998</v>
       </c>
       <c r="G67" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H67" s="33">
-        <v>2.5</v>
-      </c>
-      <c r="I67" s="33">
-        <v>0</v>
-      </c>
-      <c r="J67" s="2">
-        <v>0</v>
-      </c>
-      <c r="K67" s="4">
-        <v>2.5</v>
+        <v>29.194775510204082</v>
+      </c>
+      <c r="H67" s="38">
+        <v>5</v>
+      </c>
+      <c r="I67" s="38">
+        <v>10</v>
+      </c>
+      <c r="J67" s="15">
+        <v>0</v>
+      </c>
+      <c r="K67" s="21">
+        <v>5</v>
       </c>
       <c r="L67" s="3">
         <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="M67" s="27" t="s">
-        <v>135</v>
-      </c>
+        <v>96.194775510204082</v>
+      </c>
+      <c r="M67" s="26"/>
       <c r="IG67" s="7"/>
       <c r="IH67" s="7"/>
       <c r="II67" s="7"/>
     </row>
     <row r="68" spans="1:243" ht="25" customHeight="1">
       <c r="A68" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="B68" s="55">
-        <v>24</v>
-      </c>
-      <c r="C68" s="56"/>
-      <c r="D68" s="57"/>
+        <v>71</v>
+      </c>
+      <c r="B68" s="56">
+        <v>27</v>
+      </c>
+      <c r="C68" s="57"/>
+      <c r="D68" s="58"/>
       <c r="E68" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F68" s="40">
-        <v>0</v>
+        <v>83.125</v>
       </c>
       <c r="G68" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.443877551020408</v>
       </c>
       <c r="H68" s="33">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I68" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J68" s="2">
-        <v>1.0291E-2</v>
+        <v>0.16397200000000001</v>
       </c>
       <c r="K68" s="4">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L68" s="3">
         <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="M68" s="26" t="s">
-        <v>136</v>
-      </c>
+        <v>89.443877551020407</v>
+      </c>
+      <c r="M68" s="27"/>
       <c r="IG68" s="7"/>
       <c r="IH68" s="7"/>
       <c r="II68" s="7"/>
     </row>
     <row r="69" spans="1:243" ht="25" customHeight="1">
       <c r="A69" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="B69" s="55">
-        <v>21</v>
-      </c>
-      <c r="C69" s="56"/>
-      <c r="D69" s="57"/>
+        <v>72</v>
+      </c>
+      <c r="B69" s="56">
+        <v>30</v>
+      </c>
+      <c r="C69" s="57"/>
+      <c r="D69" s="58"/>
       <c r="E69" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F69" s="40">
-        <v>0</v>
+        <v>86.150999999999996</v>
       </c>
       <c r="G69" s="39">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12.826326530612246</v>
       </c>
       <c r="H69" s="33">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="I69" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J69" s="2">
-        <v>0</v>
+        <v>0.79987600000000003</v>
       </c>
       <c r="K69" s="4">
         <v>2.5</v>
       </c>
       <c r="L69" s="3">
         <f t="shared" si="2"/>
-        <v>26</v>
-      </c>
-      <c r="M69" s="27" t="s">
-        <v>137</v>
-      </c>
+        <v>90.326326530612249</v>
+      </c>
+      <c r="M69" s="26"/>
       <c r="IG69" s="7"/>
       <c r="IH69" s="7"/>
       <c r="II69" s="7"/>
     </row>
     <row r="70" spans="1:243" ht="25" customHeight="1">
       <c r="A70" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B70" s="55">
-        <v>24</v>
-      </c>
-      <c r="C70" s="56"/>
-      <c r="D70" s="57"/>
+        <v>73</v>
+      </c>
+      <c r="B70" s="56">
+        <v>30</v>
+      </c>
+      <c r="C70" s="57"/>
+      <c r="D70" s="58"/>
       <c r="E70" s="33">
         <v>30</v>
       </c>
       <c r="F70" s="40">
-        <v>82.278999999999996</v>
+        <v>11.093</v>
       </c>
       <c r="G70" s="39">
         <f t="shared" si="1"/>
-        <v>13.616530612244899</v>
+        <v>28.144285714285715</v>
       </c>
       <c r="H70" s="33">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="I70" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J70" s="2">
-        <v>3.6273E-2</v>
+        <v>5.2023E-2</v>
       </c>
       <c r="K70" s="4">
         <v>2.5</v>
       </c>
       <c r="L70" s="3">
         <f t="shared" si="2"/>
-        <v>74.616530612244901</v>
-      </c>
-      <c r="M70" s="26" t="s">
-        <v>138</v>
+        <v>100</v>
+      </c>
+      <c r="M70" s="25" t="s">
+        <v>133</v>
       </c>
       <c r="IG70" s="7"/>
       <c r="IH70" s="7"/>
@@ -7796,25 +7858,25 @@
     </row>
     <row r="71" spans="1:243" ht="25" customHeight="1">
       <c r="A71" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="B71" s="55">
-        <v>27</v>
-      </c>
-      <c r="C71" s="56"/>
-      <c r="D71" s="57"/>
+        <v>74</v>
+      </c>
+      <c r="B71" s="56">
+        <v>24</v>
+      </c>
+      <c r="C71" s="57"/>
+      <c r="D71" s="58"/>
       <c r="E71" s="33">
         <v>30</v>
       </c>
       <c r="F71" s="40">
-        <v>85.936999999999998</v>
+        <v>157.71</v>
       </c>
       <c r="G71" s="39">
         <f t="shared" si="1"/>
-        <v>12.870000000000001</v>
+        <v>10</v>
       </c>
       <c r="H71" s="33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I71" s="33">
         <v>0</v>
@@ -7827,10 +7889,10 @@
       </c>
       <c r="L71" s="3">
         <f t="shared" si="2"/>
-        <v>76.37</v>
-      </c>
-      <c r="M71" s="27" t="s">
-        <v>139</v>
+        <v>71.5</v>
+      </c>
+      <c r="M71" s="26" t="s">
+        <v>134</v>
       </c>
       <c r="IG71" s="7"/>
       <c r="IH71" s="7"/>
@@ -7838,25 +7900,25 @@
     </row>
     <row r="72" spans="1:243" ht="25" customHeight="1">
       <c r="A72" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="B72" s="55">
+        <v>75</v>
+      </c>
+      <c r="B72" s="56">
         <v>24</v>
       </c>
-      <c r="C72" s="56"/>
-      <c r="D72" s="57"/>
+      <c r="C72" s="57"/>
+      <c r="D72" s="58"/>
       <c r="E72" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F72" s="40">
-        <v>160.13</v>
+        <v>0</v>
       </c>
       <c r="G72" s="39">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H72" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I72" s="33">
         <v>0</v>
@@ -7869,10 +7931,10 @@
       </c>
       <c r="L72" s="3">
         <f t="shared" si="2"/>
-        <v>71</v>
-      </c>
-      <c r="M72" s="26" t="s">
-        <v>140</v>
+        <v>29</v>
+      </c>
+      <c r="M72" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="IG72" s="7"/>
       <c r="IH72" s="7"/>
@@ -7880,13 +7942,13 @@
     </row>
     <row r="73" spans="1:243" ht="25" customHeight="1">
       <c r="A73" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B73" s="55">
-        <v>21</v>
-      </c>
-      <c r="C73" s="56"/>
-      <c r="D73" s="57"/>
+        <v>76</v>
+      </c>
+      <c r="B73" s="56">
+        <v>24</v>
+      </c>
+      <c r="C73" s="57"/>
+      <c r="D73" s="58"/>
       <c r="E73" s="33">
         <v>0</v>
       </c>
@@ -7894,7 +7956,7 @@
         <v>0</v>
       </c>
       <c r="G73" s="39">
-        <f t="shared" ref="G73:G113" si="3">IF(F73&gt;0, IF(F73&lt;2, 30, IF(F73&gt;100, 10, (1-(F73-2)/(100-2))*20+10)), 0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H73" s="33">
@@ -7904,17 +7966,17 @@
         <v>0</v>
       </c>
       <c r="J73" s="2">
-        <v>8.7390000000000002E-3</v>
+        <v>1.0291E-2</v>
       </c>
       <c r="K73" s="4">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="L73" s="3">
         <f t="shared" si="2"/>
-        <v>27.5</v>
-      </c>
-      <c r="M73" s="27" t="s">
-        <v>141</v>
+        <v>29</v>
+      </c>
+      <c r="M73" s="26" t="s">
+        <v>136</v>
       </c>
       <c r="IG73" s="7"/>
       <c r="IH73" s="7"/>
@@ -7922,28 +7984,28 @@
     </row>
     <row r="74" spans="1:243" ht="25" customHeight="1">
       <c r="A74" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B74" s="55">
-        <v>30</v>
-      </c>
-      <c r="C74" s="56"/>
-      <c r="D74" s="57"/>
+        <v>77</v>
+      </c>
+      <c r="B74" s="56">
+        <v>21</v>
+      </c>
+      <c r="C74" s="57"/>
+      <c r="D74" s="58"/>
       <c r="E74" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F74" s="40">
-        <v>22.228999999999999</v>
+        <v>0</v>
       </c>
       <c r="G74" s="39">
-        <f t="shared" si="3"/>
-        <v>25.871632653061226</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="H74" s="33">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="I74" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J74" s="2">
         <v>0</v>
@@ -7953,50 +8015,52 @@
       </c>
       <c r="L74" s="3">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="M74" s="26"/>
+        <v>26</v>
+      </c>
+      <c r="M74" s="27" t="s">
+        <v>137</v>
+      </c>
       <c r="IG74" s="7"/>
       <c r="IH74" s="7"/>
       <c r="II74" s="7"/>
     </row>
     <row r="75" spans="1:243" ht="25" customHeight="1">
       <c r="A75" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B75" s="55">
-        <v>27</v>
-      </c>
-      <c r="C75" s="56"/>
-      <c r="D75" s="57"/>
+        <v>78</v>
+      </c>
+      <c r="B75" s="56">
+        <v>24</v>
+      </c>
+      <c r="C75" s="57"/>
+      <c r="D75" s="58"/>
       <c r="E75" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F75" s="40">
-        <v>0</v>
+        <v>82.278999999999996</v>
       </c>
       <c r="G75" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>13.616530612244899</v>
       </c>
       <c r="H75" s="33">
+        <v>4.5</v>
+      </c>
+      <c r="I75" s="33">
+        <v>0</v>
+      </c>
+      <c r="J75" s="2">
+        <v>3.6273E-2</v>
+      </c>
+      <c r="K75" s="4">
         <v>2.5</v>
-      </c>
-      <c r="I75" s="33">
-        <v>0</v>
-      </c>
-      <c r="J75" s="2">
-        <v>0.25622400000000001</v>
-      </c>
-      <c r="K75" s="4">
-        <v>4.5</v>
       </c>
       <c r="L75" s="3">
         <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="M75" s="27" t="s">
-        <v>135</v>
+        <v>74.616530612244901</v>
+      </c>
+      <c r="M75" s="26" t="s">
+        <v>138</v>
       </c>
       <c r="IG75" s="7"/>
       <c r="IH75" s="7"/>
@@ -8004,28 +8068,28 @@
     </row>
     <row r="76" spans="1:243" ht="25" customHeight="1">
       <c r="A76" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="B76" s="55">
-        <v>30</v>
-      </c>
-      <c r="C76" s="56"/>
-      <c r="D76" s="57"/>
+        <v>79</v>
+      </c>
+      <c r="B76" s="56">
+        <v>27</v>
+      </c>
+      <c r="C76" s="57"/>
+      <c r="D76" s="58"/>
       <c r="E76" s="33">
         <v>30</v>
       </c>
       <c r="F76" s="40">
-        <v>22.785</v>
+        <v>85.936999999999998</v>
       </c>
       <c r="G76" s="39">
-        <f t="shared" si="3"/>
-        <v>25.758163265306123</v>
+        <f t="shared" si="1"/>
+        <v>12.870000000000001</v>
       </c>
       <c r="H76" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I76" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J76" s="2">
         <v>0</v>
@@ -8035,50 +8099,52 @@
       </c>
       <c r="L76" s="3">
         <f t="shared" si="2"/>
-        <v>100</v>
-      </c>
-      <c r="M76" s="26"/>
+        <v>76.37</v>
+      </c>
+      <c r="M76" s="27" t="s">
+        <v>139</v>
+      </c>
       <c r="IG76" s="7"/>
       <c r="IH76" s="7"/>
       <c r="II76" s="7"/>
     </row>
     <row r="77" spans="1:243" ht="25" customHeight="1">
       <c r="A77" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="B77" s="55">
+        <v>80</v>
+      </c>
+      <c r="B77" s="56">
         <v>24</v>
       </c>
-      <c r="C77" s="56"/>
-      <c r="D77" s="57"/>
+      <c r="C77" s="57"/>
+      <c r="D77" s="58"/>
       <c r="E77" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F77" s="40">
-        <v>0</v>
+        <v>160.13</v>
       </c>
       <c r="G77" s="39">
-        <f t="shared" si="3"/>
-        <v>0</v>
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
       <c r="H77" s="33">
+        <v>4.5</v>
+      </c>
+      <c r="I77" s="33">
+        <v>0</v>
+      </c>
+      <c r="J77" s="2">
+        <v>0</v>
+      </c>
+      <c r="K77" s="4">
         <v>2.5</v>
-      </c>
-      <c r="I77" s="33">
-        <v>0</v>
-      </c>
-      <c r="J77" s="2">
-        <v>0.25599100000000002</v>
-      </c>
-      <c r="K77" s="4">
-        <v>3.5</v>
       </c>
       <c r="L77" s="3">
         <f t="shared" si="2"/>
-        <v>30</v>
-      </c>
-      <c r="M77" s="27" t="s">
-        <v>142</v>
+        <v>71</v>
+      </c>
+      <c r="M77" s="26" t="s">
+        <v>140</v>
       </c>
       <c r="IG77" s="7"/>
       <c r="IH77" s="7"/>
@@ -8086,95 +8152,95 @@
     </row>
     <row r="78" spans="1:243" ht="25" customHeight="1">
       <c r="A78" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B78" s="55">
-        <v>24</v>
-      </c>
-      <c r="C78" s="56"/>
-      <c r="D78" s="57"/>
+        <v>81</v>
+      </c>
+      <c r="B78" s="56">
+        <v>21</v>
+      </c>
+      <c r="C78" s="57"/>
+      <c r="D78" s="58"/>
       <c r="E78" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F78" s="40">
-        <v>89.034999999999997</v>
+        <v>0</v>
       </c>
       <c r="G78" s="39">
-        <f t="shared" si="3"/>
-        <v>12.237755102040817</v>
+        <f t="shared" ref="G78:G118" si="3">IF(F78&gt;0, IF(F78&lt;2, 30, IF(F78&gt;100, 10, (1-(F78-2)/(100-2))*20+10)), 0)</f>
+        <v>0</v>
       </c>
       <c r="H78" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="I78" s="33">
+        <v>0</v>
+      </c>
+      <c r="J78" s="2">
+        <v>8.7390000000000002E-3</v>
+      </c>
+      <c r="K78" s="4">
         <v>4</v>
-      </c>
-      <c r="I78" s="33">
-        <v>10</v>
-      </c>
-      <c r="J78" s="2">
-        <v>0</v>
-      </c>
-      <c r="K78" s="4">
-        <v>2.5</v>
       </c>
       <c r="L78" s="3">
         <f t="shared" si="2"/>
-        <v>82.737755102040822</v>
-      </c>
-      <c r="M78" s="26"/>
+        <v>27.5</v>
+      </c>
+      <c r="M78" s="27" t="s">
+        <v>141</v>
+      </c>
       <c r="IG78" s="7"/>
       <c r="IH78" s="7"/>
       <c r="II78" s="7"/>
     </row>
     <row r="79" spans="1:243" ht="25" customHeight="1">
       <c r="A79" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="B79" s="55">
-        <v>27</v>
-      </c>
-      <c r="C79" s="56"/>
-      <c r="D79" s="57"/>
+        <v>82</v>
+      </c>
+      <c r="B79" s="56">
+        <v>30</v>
+      </c>
+      <c r="C79" s="57"/>
+      <c r="D79" s="58"/>
       <c r="E79" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F79" s="40">
-        <v>0</v>
+        <v>22.228999999999999</v>
       </c>
       <c r="G79" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>25.871632653061226</v>
       </c>
       <c r="H79" s="33">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I79" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J79" s="2">
-        <v>0.11136799999999999</v>
+        <v>0</v>
       </c>
       <c r="K79" s="4">
         <v>2.5</v>
       </c>
       <c r="L79" s="3">
         <f t="shared" si="2"/>
-        <v>32</v>
-      </c>
-      <c r="M79" s="27" t="s">
-        <v>142</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M79" s="26"/>
       <c r="IG79" s="7"/>
       <c r="IH79" s="7"/>
       <c r="II79" s="7"/>
     </row>
     <row r="80" spans="1:243" ht="25" customHeight="1">
       <c r="A80" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B80" s="55">
-        <v>24</v>
-      </c>
-      <c r="C80" s="56"/>
-      <c r="D80" s="57"/>
+        <v>83</v>
+      </c>
+      <c r="B80" s="56">
+        <v>27</v>
+      </c>
+      <c r="C80" s="57"/>
+      <c r="D80" s="58"/>
       <c r="E80" s="33">
         <v>0</v>
       </c>
@@ -8192,17 +8258,17 @@
         <v>0</v>
       </c>
       <c r="J80" s="2">
-        <v>0</v>
+        <v>0.25622400000000001</v>
       </c>
       <c r="K80" s="4">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L80" s="3">
         <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="M80" s="26" t="s">
-        <v>143</v>
+        <v>34</v>
+      </c>
+      <c r="M80" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="IG80" s="7"/>
       <c r="IH80" s="7"/>
@@ -8210,137 +8276,135 @@
     </row>
     <row r="81" spans="1:243" ht="25" customHeight="1">
       <c r="A81" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" s="55">
-        <v>21</v>
-      </c>
-      <c r="C81" s="56"/>
-      <c r="D81" s="57"/>
+        <v>84</v>
+      </c>
+      <c r="B81" s="56">
+        <v>30</v>
+      </c>
+      <c r="C81" s="57"/>
+      <c r="D81" s="58"/>
       <c r="E81" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F81" s="40">
-        <v>0</v>
+        <v>22.785</v>
       </c>
       <c r="G81" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>25.758163265306123</v>
       </c>
       <c r="H81" s="33">
+        <v>5</v>
+      </c>
+      <c r="I81" s="33">
+        <v>10</v>
+      </c>
+      <c r="J81" s="2">
+        <v>0</v>
+      </c>
+      <c r="K81" s="4">
         <v>2.5</v>
-      </c>
-      <c r="I81" s="33">
-        <v>0</v>
-      </c>
-      <c r="J81" s="2">
-        <v>0.23594999999999999</v>
-      </c>
-      <c r="K81" s="4">
-        <v>3.5</v>
       </c>
       <c r="L81" s="3">
         <f t="shared" si="2"/>
-        <v>27</v>
-      </c>
-      <c r="M81" s="27" t="s">
-        <v>140</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="M81" s="26"/>
       <c r="IG81" s="7"/>
       <c r="IH81" s="7"/>
       <c r="II81" s="7"/>
     </row>
     <row r="82" spans="1:243" ht="25" customHeight="1">
       <c r="A82" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B82" s="55">
+        <v>85</v>
+      </c>
+      <c r="B82" s="56">
         <v>24</v>
       </c>
-      <c r="C82" s="56"/>
-      <c r="D82" s="57"/>
+      <c r="C82" s="57"/>
+      <c r="D82" s="58"/>
       <c r="E82" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F82" s="40">
-        <v>76.835999999999999</v>
+        <v>0</v>
       </c>
       <c r="G82" s="39">
         <f t="shared" si="3"/>
-        <v>14.72734693877551</v>
+        <v>0</v>
       </c>
       <c r="H82" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I82" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J82" s="2">
-        <v>0</v>
+        <v>0.25599100000000002</v>
       </c>
       <c r="K82" s="4">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="L82" s="3">
         <f t="shared" si="2"/>
-        <v>85.727346938775511</v>
-      </c>
-      <c r="M82" s="26"/>
+        <v>30</v>
+      </c>
+      <c r="M82" s="27" t="s">
+        <v>142</v>
+      </c>
       <c r="IG82" s="7"/>
       <c r="IH82" s="7"/>
       <c r="II82" s="7"/>
     </row>
     <row r="83" spans="1:243" ht="25" customHeight="1">
       <c r="A83" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B83" s="55">
-        <v>30</v>
-      </c>
-      <c r="C83" s="56"/>
-      <c r="D83" s="57"/>
+        <v>86</v>
+      </c>
+      <c r="B83" s="56">
+        <v>24</v>
+      </c>
+      <c r="C83" s="57"/>
+      <c r="D83" s="58"/>
       <c r="E83" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F83" s="40">
-        <v>0</v>
+        <v>89.034999999999997</v>
       </c>
       <c r="G83" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>12.237755102040817</v>
       </c>
       <c r="H83" s="33">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="I83" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J83" s="2">
-        <v>1.6031E-2</v>
+        <v>0</v>
       </c>
       <c r="K83" s="4">
         <v>2.5</v>
       </c>
       <c r="L83" s="3">
         <f t="shared" si="2"/>
-        <v>35</v>
-      </c>
-      <c r="M83" s="27" t="s">
-        <v>135</v>
-      </c>
+        <v>82.737755102040822</v>
+      </c>
+      <c r="M83" s="26"/>
       <c r="IG83" s="7"/>
       <c r="IH83" s="7"/>
       <c r="II83" s="7"/>
     </row>
     <row r="84" spans="1:243" ht="25" customHeight="1">
       <c r="A84" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B84" s="55">
-        <v>24</v>
-      </c>
-      <c r="C84" s="56"/>
-      <c r="D84" s="57"/>
+        <v>87</v>
+      </c>
+      <c r="B84" s="56">
+        <v>27</v>
+      </c>
+      <c r="C84" s="57"/>
+      <c r="D84" s="58"/>
       <c r="E84" s="33">
         <v>0</v>
       </c>
@@ -8358,17 +8422,17 @@
         <v>0</v>
       </c>
       <c r="J84" s="2">
-        <v>0.36402000000000001</v>
+        <v>0.11136799999999999</v>
       </c>
       <c r="K84" s="4">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="L84" s="3">
-        <f t="shared" ref="L84:L113" si="4">IF(SUM(B84:E84,G84,H84:I84,K84)&lt;100, SUM(B84:E84,G84,H84:I84,K84),  100)</f>
-        <v>30</v>
-      </c>
-      <c r="M84" s="26" t="s">
-        <v>144</v>
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="M84" s="27" t="s">
+        <v>142</v>
       </c>
       <c r="IG84" s="7"/>
       <c r="IH84" s="7"/>
@@ -8376,173 +8440,179 @@
     </row>
     <row r="85" spans="1:243" ht="25" customHeight="1">
       <c r="A85" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B85" s="55">
-        <v>21</v>
-      </c>
-      <c r="C85" s="56"/>
-      <c r="D85" s="57"/>
+        <v>60</v>
+      </c>
+      <c r="B85" s="56">
+        <v>24</v>
+      </c>
+      <c r="C85" s="57"/>
+      <c r="D85" s="58"/>
       <c r="E85" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F85" s="40">
-        <v>76.659000000000006</v>
+        <v>0</v>
       </c>
       <c r="G85" s="39">
         <f t="shared" si="3"/>
-        <v>14.763469387755102</v>
+        <v>0</v>
       </c>
       <c r="H85" s="33">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I85" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J85" s="2">
-        <v>0.18420700000000001</v>
+        <v>0</v>
       </c>
       <c r="K85" s="4">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="L85" s="3">
-        <f t="shared" si="4"/>
-        <v>83.763469387755094</v>
-      </c>
-      <c r="M85" s="27"/>
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="M85" s="26" t="s">
+        <v>143</v>
+      </c>
       <c r="IG85" s="7"/>
       <c r="IH85" s="7"/>
       <c r="II85" s="7"/>
     </row>
     <row r="86" spans="1:243" ht="25" customHeight="1">
       <c r="A86" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B86" s="55">
-        <v>24</v>
-      </c>
-      <c r="C86" s="56"/>
-      <c r="D86" s="57"/>
+        <v>40</v>
+      </c>
+      <c r="B86" s="56">
+        <v>21</v>
+      </c>
+      <c r="C86" s="57"/>
+      <c r="D86" s="58"/>
       <c r="E86" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F86" s="40">
-        <v>75.662000000000006</v>
+        <v>0</v>
       </c>
       <c r="G86" s="39">
         <f t="shared" si="3"/>
-        <v>14.966938775510204</v>
+        <v>0</v>
       </c>
       <c r="H86" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I86" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J86" s="2">
-        <v>0.29575899999999999</v>
+        <v>0.23594999999999999</v>
       </c>
       <c r="K86" s="4">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="L86" s="3">
-        <f t="shared" si="4"/>
-        <v>88.466938775510201</v>
-      </c>
-      <c r="M86" s="26"/>
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="M86" s="27" t="s">
+        <v>140</v>
+      </c>
       <c r="IG86" s="7"/>
       <c r="IH86" s="7"/>
       <c r="II86" s="7"/>
     </row>
     <row r="87" spans="1:243" ht="25" customHeight="1">
       <c r="A87" s="11" t="s">
-        <v>91</v>
-      </c>
-      <c r="B87" s="55">
-        <v>30</v>
-      </c>
-      <c r="C87" s="56"/>
-      <c r="D87" s="57"/>
+        <v>59</v>
+      </c>
+      <c r="B87" s="56">
+        <v>24</v>
+      </c>
+      <c r="C87" s="57"/>
+      <c r="D87" s="58"/>
       <c r="E87" s="33">
         <v>30</v>
       </c>
       <c r="F87" s="40">
-        <v>18.93</v>
+        <v>76.835999999999999</v>
       </c>
       <c r="G87" s="39">
         <f t="shared" si="3"/>
-        <v>26.544897959183672</v>
+        <v>14.72734693877551</v>
       </c>
       <c r="H87" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="I87" s="33">
         <v>10</v>
       </c>
       <c r="J87" s="2">
-        <v>2.3715E-2</v>
+        <v>0</v>
       </c>
       <c r="K87" s="4">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="L87" s="3">
-        <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="M87" s="27"/>
+        <f t="shared" si="2"/>
+        <v>85.727346938775511</v>
+      </c>
+      <c r="M87" s="26"/>
       <c r="IG87" s="7"/>
       <c r="IH87" s="7"/>
       <c r="II87" s="7"/>
     </row>
     <row r="88" spans="1:243" ht="25" customHeight="1">
       <c r="A88" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B88" s="55">
-        <v>24</v>
-      </c>
-      <c r="C88" s="56"/>
-      <c r="D88" s="57"/>
+        <v>28</v>
+      </c>
+      <c r="B88" s="56">
+        <v>30</v>
+      </c>
+      <c r="C88" s="57"/>
+      <c r="D88" s="58"/>
       <c r="E88" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F88" s="40">
-        <v>19.364000000000001</v>
+        <v>0</v>
       </c>
       <c r="G88" s="39">
         <f t="shared" si="3"/>
-        <v>26.456326530612245</v>
+        <v>0</v>
       </c>
       <c r="H88" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I88" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J88" s="2">
-        <v>0</v>
+        <v>1.6031E-2</v>
       </c>
       <c r="K88" s="4">
         <v>2.5</v>
       </c>
       <c r="L88" s="3">
-        <f t="shared" si="4"/>
-        <v>97.456326530612245</v>
-      </c>
-      <c r="M88" s="26"/>
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="M88" s="27" t="s">
+        <v>135</v>
+      </c>
       <c r="IG88" s="7"/>
       <c r="IH88" s="7"/>
       <c r="II88" s="7"/>
     </row>
     <row r="89" spans="1:243" ht="25" customHeight="1">
       <c r="A89" s="11" t="s">
-        <v>93</v>
-      </c>
-      <c r="B89" s="55">
-        <v>27</v>
-      </c>
-      <c r="C89" s="56"/>
-      <c r="D89" s="57"/>
+        <v>88</v>
+      </c>
+      <c r="B89" s="56">
+        <v>24</v>
+      </c>
+      <c r="C89" s="57"/>
+      <c r="D89" s="58"/>
       <c r="E89" s="33">
         <v>0</v>
       </c>
@@ -8560,17 +8630,17 @@
         <v>0</v>
       </c>
       <c r="J89" s="2">
-        <v>0</v>
+        <v>0.36402000000000001</v>
       </c>
       <c r="K89" s="4">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="L89" s="3">
-        <f t="shared" si="4"/>
-        <v>32</v>
-      </c>
-      <c r="M89" s="27" t="s">
-        <v>142</v>
+        <f t="shared" ref="L89:L118" si="4">IF(SUM(B89:E89,G89,H89:I89,K89)&lt;100, SUM(B89:E89,G89,H89:I89,K89),  100)</f>
+        <v>30</v>
+      </c>
+      <c r="M89" s="26" t="s">
+        <v>144</v>
       </c>
       <c r="IG89" s="7"/>
       <c r="IH89" s="7"/>
@@ -8578,149 +8648,145 @@
     </row>
     <row r="90" spans="1:243" ht="25" customHeight="1">
       <c r="A90" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B90" s="55">
+        <v>89</v>
+      </c>
+      <c r="B90" s="56">
         <v>21</v>
       </c>
-      <c r="C90" s="56"/>
-      <c r="D90" s="57"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="58"/>
       <c r="E90" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F90" s="40">
-        <v>0</v>
+        <v>76.659000000000006</v>
       </c>
       <c r="G90" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.763469387755102</v>
       </c>
       <c r="H90" s="33">
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
       <c r="I90" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J90" s="2">
-        <v>0</v>
+        <v>0.18420700000000001</v>
       </c>
       <c r="K90" s="4">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L90" s="3">
         <f t="shared" si="4"/>
-        <v>26</v>
-      </c>
-      <c r="M90" s="26" t="s">
-        <v>135</v>
-      </c>
+        <v>83.763469387755094</v>
+      </c>
+      <c r="M90" s="27"/>
       <c r="IG90" s="7"/>
       <c r="IH90" s="7"/>
       <c r="II90" s="7"/>
     </row>
     <row r="91" spans="1:243" ht="25" customHeight="1">
       <c r="A91" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B91" s="55">
-        <v>27</v>
-      </c>
-      <c r="C91" s="56"/>
-      <c r="D91" s="57"/>
+        <v>90</v>
+      </c>
+      <c r="B91" s="56">
+        <v>24</v>
+      </c>
+      <c r="C91" s="57"/>
+      <c r="D91" s="58"/>
       <c r="E91" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F91" s="40">
-        <v>0</v>
+        <v>75.662000000000006</v>
       </c>
       <c r="G91" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>14.966938775510204</v>
       </c>
       <c r="H91" s="33">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I91" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J91" s="2">
-        <v>0.616757</v>
+        <v>0.29575899999999999</v>
       </c>
       <c r="K91" s="4">
-        <v>4.5</v>
+        <v>5</v>
       </c>
       <c r="L91" s="3">
         <f t="shared" si="4"/>
-        <v>34</v>
-      </c>
-      <c r="M91" s="27" t="s">
-        <v>145</v>
-      </c>
+        <v>88.466938775510201</v>
+      </c>
+      <c r="M91" s="26"/>
       <c r="IG91" s="7"/>
       <c r="IH91" s="7"/>
       <c r="II91" s="7"/>
     </row>
     <row r="92" spans="1:243" ht="25" customHeight="1">
       <c r="A92" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B92" s="55">
-        <v>30</v>
-      </c>
-      <c r="C92" s="56"/>
-      <c r="D92" s="57"/>
+        <v>91</v>
+      </c>
+      <c r="B92" s="56">
+        <v>30</v>
+      </c>
+      <c r="C92" s="57"/>
+      <c r="D92" s="58"/>
       <c r="E92" s="33">
         <v>30</v>
       </c>
       <c r="F92" s="40">
-        <v>80.263999999999996</v>
+        <v>18.93</v>
       </c>
       <c r="G92" s="39">
         <f t="shared" si="3"/>
-        <v>14.027755102040818</v>
+        <v>26.544897959183672</v>
       </c>
       <c r="H92" s="33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I92" s="33">
         <v>10</v>
       </c>
       <c r="J92" s="2">
-        <v>2.2478000000000001E-2</v>
+        <v>2.3715E-2</v>
       </c>
       <c r="K92" s="4">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="L92" s="3">
         <f t="shared" si="4"/>
-        <v>92.027755102040814</v>
-      </c>
-      <c r="M92" s="26"/>
+        <v>100</v>
+      </c>
+      <c r="M92" s="27"/>
       <c r="IG92" s="7"/>
       <c r="IH92" s="7"/>
       <c r="II92" s="7"/>
     </row>
     <row r="93" spans="1:243" ht="25" customHeight="1">
       <c r="A93" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="B93" s="55">
-        <v>21</v>
-      </c>
-      <c r="C93" s="56"/>
-      <c r="D93" s="57"/>
+        <v>92</v>
+      </c>
+      <c r="B93" s="56">
+        <v>24</v>
+      </c>
+      <c r="C93" s="57"/>
+      <c r="D93" s="58"/>
       <c r="E93" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F93" s="40">
-        <v>0</v>
+        <v>19.364000000000001</v>
       </c>
       <c r="G93" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26.456326530612245</v>
       </c>
       <c r="H93" s="33">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I93" s="33">
         <v>10</v>
@@ -8733,24 +8799,22 @@
       </c>
       <c r="L93" s="3">
         <f t="shared" si="4"/>
-        <v>36</v>
-      </c>
-      <c r="M93" s="27" t="s">
-        <v>146</v>
-      </c>
+        <v>97.456326530612245</v>
+      </c>
+      <c r="M93" s="26"/>
       <c r="IG93" s="7"/>
       <c r="IH93" s="7"/>
       <c r="II93" s="7"/>
     </row>
     <row r="94" spans="1:243" ht="25" customHeight="1">
       <c r="A94" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="B94" s="55">
-        <v>0</v>
-      </c>
-      <c r="C94" s="56"/>
-      <c r="D94" s="57"/>
+        <v>93</v>
+      </c>
+      <c r="B94" s="56">
+        <v>27</v>
+      </c>
+      <c r="C94" s="57"/>
+      <c r="D94" s="58"/>
       <c r="E94" s="33">
         <v>0</v>
       </c>
@@ -8768,17 +8832,17 @@
         <v>0</v>
       </c>
       <c r="J94" s="2">
-        <v>1.7333999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="K94" s="4">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="L94" s="3">
         <f t="shared" si="4"/>
-        <v>7</v>
-      </c>
-      <c r="M94" s="26" t="s">
-        <v>135</v>
+        <v>32</v>
+      </c>
+      <c r="M94" s="27" t="s">
+        <v>142</v>
       </c>
       <c r="IG94" s="7"/>
       <c r="IH94" s="7"/>
@@ -8786,401 +8850,420 @@
     </row>
     <row r="95" spans="1:243" ht="25" customHeight="1">
       <c r="A95" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B95" s="55">
-        <v>27</v>
-      </c>
-      <c r="C95" s="56"/>
-      <c r="D95" s="57"/>
+        <v>94</v>
+      </c>
+      <c r="B95" s="56">
+        <v>21</v>
+      </c>
+      <c r="C95" s="57"/>
+      <c r="D95" s="58"/>
       <c r="E95" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F95" s="40">
-        <v>20.995999999999999</v>
+        <v>0</v>
       </c>
       <c r="G95" s="39">
         <f t="shared" si="3"/>
-        <v>26.123265306122448</v>
+        <v>0</v>
       </c>
       <c r="H95" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I95" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J95" s="2">
-        <v>2.4060000000000002E-2</v>
+        <v>0</v>
       </c>
       <c r="K95" s="4">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="L95" s="3">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="M95" s="27"/>
+        <v>26</v>
+      </c>
+      <c r="M95" s="26" t="s">
+        <v>135</v>
+      </c>
       <c r="IG95" s="7"/>
       <c r="IH95" s="7"/>
       <c r="II95" s="7"/>
     </row>
     <row r="96" spans="1:243" ht="25" customHeight="1">
       <c r="A96" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="B96" s="55">
-        <v>21</v>
-      </c>
-      <c r="C96" s="56"/>
-      <c r="D96" s="57"/>
+        <v>95</v>
+      </c>
+      <c r="B96" s="56">
+        <v>27</v>
+      </c>
+      <c r="C96" s="57"/>
+      <c r="D96" s="58"/>
       <c r="E96" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F96" s="40">
-        <v>156</v>
+        <v>0</v>
       </c>
       <c r="G96" s="39">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H96" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="I96" s="33">
+        <v>0</v>
+      </c>
+      <c r="J96" s="2">
+        <v>0.616757</v>
+      </c>
+      <c r="K96" s="4">
         <v>4.5</v>
-      </c>
-      <c r="I96" s="33">
-        <v>10</v>
-      </c>
-      <c r="J96" s="2">
-        <v>0.197292</v>
-      </c>
-      <c r="K96" s="4">
-        <v>4</v>
       </c>
       <c r="L96" s="3">
         <f t="shared" si="4"/>
-        <v>79.5</v>
-      </c>
-      <c r="M96" s="26"/>
+        <v>34</v>
+      </c>
+      <c r="M96" s="27" t="s">
+        <v>145</v>
+      </c>
       <c r="IG96" s="7"/>
       <c r="IH96" s="7"/>
       <c r="II96" s="7"/>
     </row>
     <row r="97" spans="1:243" ht="25" customHeight="1">
       <c r="A97" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B97" s="55">
-        <v>24</v>
-      </c>
-      <c r="C97" s="56"/>
-      <c r="D97" s="57"/>
+        <v>31</v>
+      </c>
+      <c r="B97" s="56">
+        <v>30</v>
+      </c>
+      <c r="C97" s="57"/>
+      <c r="D97" s="58"/>
       <c r="E97" s="33">
         <v>30</v>
       </c>
       <c r="F97" s="40">
-        <v>78.983999999999995</v>
+        <v>80.263999999999996</v>
       </c>
       <c r="G97" s="39">
         <f t="shared" si="3"/>
-        <v>14.288979591836737</v>
+        <v>14.027755102040818</v>
       </c>
       <c r="H97" s="33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I97" s="33">
         <v>10</v>
       </c>
       <c r="J97" s="2">
-        <v>2.8327999999999999E-2</v>
+        <v>2.2478000000000001E-2</v>
       </c>
       <c r="K97" s="4">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="L97" s="3">
         <f t="shared" si="4"/>
-        <v>87.788979591836735</v>
-      </c>
-      <c r="M97" s="27"/>
+        <v>92.027755102040814</v>
+      </c>
+      <c r="M97" s="26"/>
       <c r="IG97" s="7"/>
       <c r="IH97" s="7"/>
       <c r="II97" s="7"/>
     </row>
     <row r="98" spans="1:243" ht="25" customHeight="1">
       <c r="A98" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B98" s="55">
-        <v>30</v>
-      </c>
-      <c r="C98" s="56"/>
-      <c r="D98" s="57"/>
+        <v>61</v>
+      </c>
+      <c r="B98" s="56">
+        <v>21</v>
+      </c>
+      <c r="C98" s="57"/>
+      <c r="D98" s="58"/>
       <c r="E98" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F98" s="40">
-        <v>158.24</v>
+        <v>0</v>
       </c>
       <c r="G98" s="39">
         <f t="shared" si="3"/>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="H98" s="33">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="I98" s="33">
         <v>10</v>
       </c>
       <c r="J98" s="2">
-        <v>0.44423499999999999</v>
+        <v>0</v>
       </c>
       <c r="K98" s="4">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="L98" s="3">
         <f t="shared" si="4"/>
-        <v>89.5</v>
-      </c>
-      <c r="M98" s="26"/>
+        <v>36</v>
+      </c>
+      <c r="M98" s="27" t="s">
+        <v>146</v>
+      </c>
       <c r="IG98" s="7"/>
       <c r="IH98" s="7"/>
       <c r="II98" s="7"/>
     </row>
     <row r="99" spans="1:243" ht="25" customHeight="1">
       <c r="A99" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B99" s="55">
-        <v>30</v>
-      </c>
-      <c r="C99" s="56"/>
-      <c r="D99" s="57"/>
+        <v>96</v>
+      </c>
+      <c r="B99" s="56">
+        <v>0</v>
+      </c>
+      <c r="C99" s="57"/>
+      <c r="D99" s="58"/>
       <c r="E99" s="33">
-        <v>30</v>
+        <v>0</v>
       </c>
       <c r="F99" s="40">
-        <v>80.319000000000003</v>
+        <v>0</v>
       </c>
       <c r="G99" s="39">
         <f t="shared" si="3"/>
-        <v>14.016530612244898</v>
+        <v>0</v>
       </c>
       <c r="H99" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I99" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J99" s="2">
-        <v>0.33158300000000002</v>
+        <v>1.7333999999999999E-2</v>
       </c>
       <c r="K99" s="4">
         <v>4.5</v>
       </c>
       <c r="L99" s="3">
         <f t="shared" si="4"/>
-        <v>93.016530612244892</v>
-      </c>
-      <c r="M99" s="27"/>
+        <v>7</v>
+      </c>
+      <c r="M99" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="IG99" s="7"/>
+      <c r="IH99" s="7"/>
+      <c r="II99" s="7"/>
     </row>
     <row r="100" spans="1:243" ht="25" customHeight="1">
       <c r="A100" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B100" s="55">
-        <v>21</v>
-      </c>
-      <c r="C100" s="56"/>
-      <c r="D100" s="57"/>
+        <v>97</v>
+      </c>
+      <c r="B100" s="56">
+        <v>27</v>
+      </c>
+      <c r="C100" s="57"/>
+      <c r="D100" s="58"/>
       <c r="E100" s="33">
         <v>30</v>
       </c>
       <c r="F100" s="40">
-        <v>0</v>
+        <v>20.995999999999999</v>
       </c>
       <c r="G100" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>26.123265306122448</v>
       </c>
       <c r="H100" s="33">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I100" s="33">
         <v>10</v>
       </c>
       <c r="J100" s="2">
-        <v>8.4103999999999998E-2</v>
+        <v>2.4060000000000002E-2</v>
       </c>
       <c r="K100" s="4">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="L100" s="3">
         <f t="shared" si="4"/>
-        <v>67</v>
-      </c>
-      <c r="M100" s="26"/>
+        <v>100</v>
+      </c>
+      <c r="M100" s="27"/>
+      <c r="IG100" s="7"/>
+      <c r="IH100" s="7"/>
+      <c r="II100" s="7"/>
     </row>
     <row r="101" spans="1:243" ht="25" customHeight="1">
       <c r="A101" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B101" s="55">
+        <v>37</v>
+      </c>
+      <c r="B101" s="56">
         <v>21</v>
       </c>
-      <c r="C101" s="56"/>
-      <c r="D101" s="57"/>
+      <c r="C101" s="57"/>
+      <c r="D101" s="58"/>
       <c r="E101" s="33">
-        <v>17.751479289940828</v>
+        <v>30</v>
       </c>
       <c r="F101" s="40">
-        <v>152.19</v>
+        <v>156</v>
       </c>
       <c r="G101" s="39">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="H101" s="33">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="I101" s="33">
         <v>10</v>
       </c>
       <c r="J101" s="2">
-        <v>1.9650999999999998E-2</v>
+        <v>0.197292</v>
       </c>
       <c r="K101" s="4">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="L101" s="3">
         <f t="shared" si="4"/>
-        <v>63.751479289940832</v>
-      </c>
-      <c r="M101" s="27"/>
+        <v>79.5</v>
+      </c>
+      <c r="M101" s="26"/>
+      <c r="IG101" s="7"/>
+      <c r="IH101" s="7"/>
+      <c r="II101" s="7"/>
     </row>
     <row r="102" spans="1:243" ht="25" customHeight="1">
       <c r="A102" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B102" s="55">
-        <v>21</v>
-      </c>
-      <c r="C102" s="56"/>
-      <c r="D102" s="57"/>
+        <v>98</v>
+      </c>
+      <c r="B102" s="56">
+        <v>24</v>
+      </c>
+      <c r="C102" s="57"/>
+      <c r="D102" s="58"/>
       <c r="E102" s="33">
-        <v>29.822485207100591</v>
+        <v>30</v>
       </c>
       <c r="F102" s="40">
-        <v>36.862000000000002</v>
+        <v>78.983999999999995</v>
       </c>
       <c r="G102" s="39">
         <f t="shared" si="3"/>
-        <v>22.885306122448981</v>
+        <v>14.288979591836737</v>
       </c>
       <c r="H102" s="33">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="I102" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J102" s="2">
-        <v>9.5962000000000006E-2</v>
+        <v>2.8327999999999999E-2</v>
       </c>
       <c r="K102" s="4">
         <v>4.5</v>
       </c>
       <c r="L102" s="3">
         <f t="shared" si="4"/>
-        <v>80.707791329549565</v>
-      </c>
-      <c r="M102" s="26" t="s">
-        <v>147</v>
-      </c>
+        <v>87.788979591836735</v>
+      </c>
+      <c r="M102" s="27"/>
+      <c r="IG102" s="7"/>
+      <c r="IH102" s="7"/>
+      <c r="II102" s="7"/>
     </row>
     <row r="103" spans="1:243" ht="25" customHeight="1">
       <c r="A103" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B103" s="55">
-        <v>24</v>
-      </c>
-      <c r="C103" s="56"/>
-      <c r="D103" s="57"/>
+        <v>99</v>
+      </c>
+      <c r="B103" s="56">
+        <v>30</v>
+      </c>
+      <c r="C103" s="57"/>
+      <c r="D103" s="58"/>
       <c r="E103" s="33">
         <v>30</v>
       </c>
       <c r="F103" s="40">
-        <v>1.0976999999999999</v>
+        <v>158.24</v>
       </c>
       <c r="G103" s="39">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H103" s="33">
+        <v>5</v>
+      </c>
+      <c r="I103" s="33">
+        <v>10</v>
+      </c>
+      <c r="J103" s="2">
+        <v>0.44423499999999999</v>
+      </c>
+      <c r="K103" s="4">
         <v>4.5</v>
-      </c>
-      <c r="I103" s="33">
-        <v>10</v>
-      </c>
-      <c r="J103" s="2">
-        <v>0.11998499999999999</v>
-      </c>
-      <c r="K103" s="4">
-        <v>2.5</v>
       </c>
       <c r="L103" s="3">
         <f t="shared" si="4"/>
-        <v>100</v>
-      </c>
-      <c r="M103" s="27"/>
+        <v>89.5</v>
+      </c>
+      <c r="M103" s="26"/>
+      <c r="IG103" s="7"/>
+      <c r="IH103" s="7"/>
+      <c r="II103" s="7"/>
     </row>
     <row r="104" spans="1:243" ht="25" customHeight="1">
       <c r="A104" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B104" s="55">
-        <v>27</v>
-      </c>
-      <c r="C104" s="56"/>
-      <c r="D104" s="57"/>
+        <v>100</v>
+      </c>
+      <c r="B104" s="56">
+        <v>30</v>
+      </c>
+      <c r="C104" s="57"/>
+      <c r="D104" s="58"/>
       <c r="E104" s="33">
         <v>30</v>
       </c>
       <c r="F104" s="40">
-        <v>83.876000000000005</v>
+        <v>80.319000000000003</v>
       </c>
       <c r="G104" s="39">
         <f t="shared" si="3"/>
-        <v>13.290612244897959</v>
+        <v>14.016530612244898</v>
       </c>
       <c r="H104" s="33">
         <v>4.5</v>
       </c>
       <c r="I104" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J104" s="2">
-        <v>0</v>
+        <v>0.33158300000000002</v>
       </c>
       <c r="K104" s="4">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L104" s="3">
         <f t="shared" si="4"/>
-        <v>77.290612244897957</v>
-      </c>
-      <c r="M104" s="26" t="s">
-        <v>139</v>
-      </c>
+        <v>93.016530612244892</v>
+      </c>
+      <c r="M104" s="27"/>
     </row>
     <row r="105" spans="1:243" ht="25" customHeight="1">
       <c r="A105" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B105" s="55">
-        <v>24</v>
-      </c>
-      <c r="C105" s="56"/>
-      <c r="D105" s="57"/>
+        <v>101</v>
+      </c>
+      <c r="B105" s="56">
+        <v>21</v>
+      </c>
+      <c r="C105" s="57"/>
+      <c r="D105" s="58"/>
       <c r="E105" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F105" s="40">
         <v>0</v>
@@ -9193,114 +9276,114 @@
         <v>2.5</v>
       </c>
       <c r="I105" s="33">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J105" s="2">
-        <v>1.952367</v>
+        <v>8.4103999999999998E-2</v>
       </c>
       <c r="K105" s="4">
-        <v>4.5</v>
+        <v>3.5</v>
       </c>
       <c r="L105" s="3">
         <f t="shared" si="4"/>
-        <v>31</v>
-      </c>
-      <c r="M105" s="27" t="s">
-        <v>148</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="M105" s="26"/>
     </row>
     <row r="106" spans="1:243" ht="25" customHeight="1">
       <c r="A106" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B106" s="55">
-        <v>27</v>
-      </c>
-      <c r="C106" s="56"/>
-      <c r="D106" s="57"/>
+        <v>102</v>
+      </c>
+      <c r="B106" s="56">
+        <v>21</v>
+      </c>
+      <c r="C106" s="57"/>
+      <c r="D106" s="58"/>
       <c r="E106" s="33">
-        <v>30</v>
+        <v>17.751479289940828</v>
       </c>
       <c r="F106" s="40">
-        <v>153.26</v>
+        <v>152.19</v>
       </c>
       <c r="G106" s="39">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="H106" s="33">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="I106" s="33">
         <v>10</v>
       </c>
       <c r="J106" s="2">
-        <v>0.29591299999999998</v>
+        <v>1.9650999999999998E-2</v>
       </c>
       <c r="K106" s="4">
-        <v>4.5</v>
+        <v>2.5</v>
       </c>
       <c r="L106" s="3">
         <f t="shared" si="4"/>
-        <v>86</v>
-      </c>
-      <c r="M106" s="26"/>
+        <v>63.751479289940832</v>
+      </c>
+      <c r="M106" s="27"/>
     </row>
     <row r="107" spans="1:243" ht="25" customHeight="1">
       <c r="A107" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B107" s="55">
-        <v>30</v>
-      </c>
-      <c r="C107" s="56"/>
-      <c r="D107" s="57"/>
+        <v>103</v>
+      </c>
+      <c r="B107" s="56">
+        <v>21</v>
+      </c>
+      <c r="C107" s="57"/>
+      <c r="D107" s="58"/>
       <c r="E107" s="33">
-        <v>30</v>
+        <v>29.822485207100591</v>
       </c>
       <c r="F107" s="40">
-        <v>74.911000000000001</v>
+        <v>36.862000000000002</v>
       </c>
       <c r="G107" s="39">
         <f t="shared" si="3"/>
-        <v>15.120204081632654</v>
+        <v>22.885306122448981</v>
       </c>
       <c r="H107" s="33">
+        <v>2.5</v>
+      </c>
+      <c r="I107" s="33">
+        <v>0</v>
+      </c>
+      <c r="J107" s="2">
+        <v>9.5962000000000006E-2</v>
+      </c>
+      <c r="K107" s="4">
         <v>4.5</v>
-      </c>
-      <c r="I107" s="33">
-        <v>10</v>
-      </c>
-      <c r="J107" s="2">
-        <v>1.5566E-2</v>
-      </c>
-      <c r="K107" s="4">
-        <v>4</v>
       </c>
       <c r="L107" s="3">
         <f t="shared" si="4"/>
-        <v>93.62020408163265</v>
-      </c>
-      <c r="M107" s="27"/>
+        <v>80.707791329549565</v>
+      </c>
+      <c r="M107" s="26" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="108" spans="1:243" ht="25" customHeight="1">
       <c r="A108" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B108" s="55">
-        <v>21</v>
-      </c>
-      <c r="C108" s="56"/>
-      <c r="D108" s="57"/>
+        <v>104</v>
+      </c>
+      <c r="B108" s="56">
+        <v>24</v>
+      </c>
+      <c r="C108" s="57"/>
+      <c r="D108" s="58"/>
       <c r="E108" s="33">
         <v>30</v>
       </c>
       <c r="F108" s="40">
-        <v>11.08</v>
+        <v>1.0976999999999999</v>
       </c>
       <c r="G108" s="39">
         <f t="shared" si="3"/>
-        <v>28.146938775510204</v>
+        <v>30</v>
       </c>
       <c r="H108" s="33">
         <v>4.5</v>
@@ -9309,65 +9392,65 @@
         <v>10</v>
       </c>
       <c r="J108" s="2">
-        <v>7.6779999999999999E-3</v>
+        <v>0.11998499999999999</v>
       </c>
       <c r="K108" s="4">
         <v>2.5</v>
       </c>
       <c r="L108" s="3">
         <f t="shared" si="4"/>
-        <v>96.146938775510208</v>
-      </c>
-      <c r="M108" s="26"/>
+        <v>100</v>
+      </c>
+      <c r="M108" s="27"/>
     </row>
     <row r="109" spans="1:243" ht="25" customHeight="1">
       <c r="A109" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B109" s="55">
-        <v>24</v>
-      </c>
-      <c r="C109" s="56"/>
-      <c r="D109" s="57"/>
+        <v>105</v>
+      </c>
+      <c r="B109" s="56">
+        <v>27</v>
+      </c>
+      <c r="C109" s="57"/>
+      <c r="D109" s="58"/>
       <c r="E109" s="33">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F109" s="40">
-        <v>0</v>
+        <v>83.876000000000005</v>
       </c>
       <c r="G109" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>13.290612244897959</v>
       </c>
       <c r="H109" s="33">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="I109" s="33">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J109" s="2">
         <v>0</v>
       </c>
       <c r="K109" s="4">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="L109" s="3">
         <f t="shared" si="4"/>
-        <v>38</v>
-      </c>
-      <c r="M109" s="27" t="s">
-        <v>165</v>
+        <v>77.290612244897957</v>
+      </c>
+      <c r="M109" s="26" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="110" spans="1:243" ht="25" customHeight="1">
       <c r="A110" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B110" s="55">
-        <v>15</v>
-      </c>
-      <c r="C110" s="56"/>
-      <c r="D110" s="57"/>
+        <v>106</v>
+      </c>
+      <c r="B110" s="56">
+        <v>24</v>
+      </c>
+      <c r="C110" s="57"/>
+      <c r="D110" s="58"/>
       <c r="E110" s="33">
         <v>0</v>
       </c>
@@ -9379,331 +9462,410 @@
         <v>0</v>
       </c>
       <c r="H110" s="33">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="I110" s="33">
         <v>0</v>
       </c>
       <c r="J110" s="2">
-        <v>7.175E-3</v>
+        <v>1.952367</v>
       </c>
       <c r="K110" s="4">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="L110" s="3">
         <f t="shared" si="4"/>
-        <v>21</v>
-      </c>
-      <c r="M110" s="26" t="s">
-        <v>166</v>
+        <v>31</v>
+      </c>
+      <c r="M110" s="27" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="111" spans="1:243" ht="25" customHeight="1">
       <c r="A111" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B111" s="55">
-        <v>21</v>
-      </c>
-      <c r="C111" s="56"/>
-      <c r="D111" s="57"/>
+        <v>107</v>
+      </c>
+      <c r="B111" s="56">
+        <v>27</v>
+      </c>
+      <c r="C111" s="57"/>
+      <c r="D111" s="58"/>
       <c r="E111" s="33">
         <v>30</v>
       </c>
       <c r="F111" s="40">
-        <v>0</v>
+        <v>153.26</v>
       </c>
       <c r="G111" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="H111" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="I111" s="33">
         <v>10</v>
       </c>
       <c r="J111" s="2">
-        <v>6.9841E-2</v>
+        <v>0.29591299999999998</v>
       </c>
       <c r="K111" s="4">
-        <v>2.2928994082840237</v>
+        <v>4.5</v>
       </c>
       <c r="L111" s="3">
         <f t="shared" si="4"/>
-        <v>68.292899408284029</v>
-      </c>
-      <c r="M111" s="27" t="s">
-        <v>167</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="M111" s="26"/>
     </row>
     <row r="112" spans="1:243" ht="25" customHeight="1">
       <c r="A112" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B112" s="55">
-        <v>21</v>
-      </c>
-      <c r="C112" s="56"/>
-      <c r="D112" s="57"/>
+        <v>108</v>
+      </c>
+      <c r="B112" s="56">
+        <v>30</v>
+      </c>
+      <c r="C112" s="57"/>
+      <c r="D112" s="58"/>
       <c r="E112" s="33">
         <v>30</v>
       </c>
       <c r="F112" s="40">
-        <v>15.122</v>
+        <v>74.911000000000001</v>
       </c>
       <c r="G112" s="39">
         <f t="shared" si="3"/>
-        <v>27.322040816326528</v>
+        <v>15.120204081632654</v>
       </c>
       <c r="H112" s="33">
         <v>4.5</v>
       </c>
       <c r="I112" s="33">
-        <v>9.1715976331360949</v>
+        <v>10</v>
       </c>
       <c r="J112" s="2">
-        <v>2.3165999999999999E-2</v>
+        <v>1.5566E-2</v>
       </c>
       <c r="K112" s="4">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="L112" s="3">
         <f t="shared" si="4"/>
-        <v>94.493638449462622</v>
-      </c>
-      <c r="M112" s="26"/>
+        <v>93.62020408163265</v>
+      </c>
+      <c r="M112" s="27"/>
     </row>
     <row r="113" spans="1:243" ht="25" customHeight="1">
       <c r="A113" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B113" s="55">
-        <v>27</v>
-      </c>
-      <c r="C113" s="56"/>
-      <c r="D113" s="57"/>
+        <v>109</v>
+      </c>
+      <c r="B113" s="56">
+        <v>21</v>
+      </c>
+      <c r="C113" s="57"/>
+      <c r="D113" s="58"/>
       <c r="E113" s="33">
-        <v>29.644970414201186</v>
+        <v>30</v>
       </c>
       <c r="F113" s="40">
-        <v>11.878</v>
+        <v>11.08</v>
       </c>
       <c r="G113" s="39">
         <f t="shared" si="3"/>
-        <v>27.984081632653062</v>
+        <v>28.146938775510204</v>
       </c>
       <c r="H113" s="33">
-        <v>5</v>
+        <v>4.5</v>
       </c>
       <c r="I113" s="33">
         <v>10</v>
       </c>
       <c r="J113" s="2">
-        <v>0</v>
+        <v>7.6779999999999999E-3</v>
       </c>
       <c r="K113" s="4">
-        <v>5</v>
+        <v>2.5</v>
       </c>
       <c r="L113" s="3">
         <f t="shared" si="4"/>
+        <v>96.146938775510208</v>
+      </c>
+      <c r="M113" s="26"/>
+    </row>
+    <row r="114" spans="1:243" ht="25" customHeight="1">
+      <c r="A114" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B114" s="56">
+        <v>24</v>
+      </c>
+      <c r="C114" s="57"/>
+      <c r="D114" s="58"/>
+      <c r="E114" s="33">
+        <v>0</v>
+      </c>
+      <c r="F114" s="40">
+        <v>0</v>
+      </c>
+      <c r="G114" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H114" s="33">
+        <v>4</v>
+      </c>
+      <c r="I114" s="33">
+        <v>10</v>
+      </c>
+      <c r="J114" s="2">
+        <v>0</v>
+      </c>
+      <c r="K114" s="4">
+        <v>0</v>
+      </c>
+      <c r="L114" s="3">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="M114" s="27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="115" spans="1:243" ht="25" customHeight="1">
+      <c r="A115" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B115" s="56">
+        <v>15</v>
+      </c>
+      <c r="C115" s="57"/>
+      <c r="D115" s="58"/>
+      <c r="E115" s="33">
+        <v>0</v>
+      </c>
+      <c r="F115" s="40">
+        <v>0</v>
+      </c>
+      <c r="G115" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H115" s="33">
+        <v>3.5</v>
+      </c>
+      <c r="I115" s="33">
+        <v>0</v>
+      </c>
+      <c r="J115" s="2">
+        <v>7.175E-3</v>
+      </c>
+      <c r="K115" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L115" s="3">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="M115" s="26" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="116" spans="1:243" ht="25" customHeight="1">
+      <c r="A116" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B116" s="56">
+        <v>21</v>
+      </c>
+      <c r="C116" s="57"/>
+      <c r="D116" s="58"/>
+      <c r="E116" s="33">
+        <v>30</v>
+      </c>
+      <c r="F116" s="40">
+        <v>0</v>
+      </c>
+      <c r="G116" s="39">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H116" s="33">
+        <v>5</v>
+      </c>
+      <c r="I116" s="33">
+        <v>10</v>
+      </c>
+      <c r="J116" s="2">
+        <v>6.9841E-2</v>
+      </c>
+      <c r="K116" s="4">
+        <v>2.2928994082840237</v>
+      </c>
+      <c r="L116" s="3">
+        <f t="shared" si="4"/>
+        <v>68.292899408284029</v>
+      </c>
+      <c r="M116" s="27" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="117" spans="1:243" ht="25" customHeight="1">
+      <c r="A117" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B117" s="56">
+        <v>21</v>
+      </c>
+      <c r="C117" s="57"/>
+      <c r="D117" s="58"/>
+      <c r="E117" s="33">
+        <v>30</v>
+      </c>
+      <c r="F117" s="40">
+        <v>15.122</v>
+      </c>
+      <c r="G117" s="39">
+        <f t="shared" si="3"/>
+        <v>27.322040816326528</v>
+      </c>
+      <c r="H117" s="33">
+        <v>4.5</v>
+      </c>
+      <c r="I117" s="33">
+        <v>9.1715976331360949</v>
+      </c>
+      <c r="J117" s="2">
+        <v>2.3165999999999999E-2</v>
+      </c>
+      <c r="K117" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="L117" s="3">
+        <f t="shared" si="4"/>
+        <v>94.493638449462622</v>
+      </c>
+      <c r="M117" s="26"/>
+    </row>
+    <row r="118" spans="1:243" ht="25" customHeight="1">
+      <c r="A118" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B118" s="56">
+        <v>27</v>
+      </c>
+      <c r="C118" s="57"/>
+      <c r="D118" s="58"/>
+      <c r="E118" s="33">
+        <v>29.644970414201186</v>
+      </c>
+      <c r="F118" s="40">
+        <v>11.878</v>
+      </c>
+      <c r="G118" s="39">
+        <f t="shared" si="3"/>
+        <v>27.984081632653062</v>
+      </c>
+      <c r="H118" s="33">
+        <v>5</v>
+      </c>
+      <c r="I118" s="33">
+        <v>10</v>
+      </c>
+      <c r="J118" s="2">
+        <v>0</v>
+      </c>
+      <c r="K118" s="4">
+        <v>5</v>
+      </c>
+      <c r="L118" s="3">
+        <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="M113" s="27"/>
-    </row>
-    <row r="114" spans="1:243" ht="25" customHeight="1">
-      <c r="A114" s="29"/>
-      <c r="B114" s="30"/>
-      <c r="C114" s="30"/>
-      <c r="D114" s="30"/>
-      <c r="E114" s="41"/>
-      <c r="F114" s="42"/>
-      <c r="G114" s="43"/>
-      <c r="H114" s="41"/>
-      <c r="I114" s="41"/>
-    </row>
-    <row r="115" spans="1:243" ht="25" customHeight="1">
-      <c r="A115" s="29"/>
-      <c r="B115" s="30"/>
-      <c r="C115" s="30"/>
-      <c r="D115" s="30"/>
-      <c r="E115" s="41"/>
-      <c r="F115" s="42"/>
-      <c r="G115" s="43"/>
-      <c r="H115" s="41"/>
-      <c r="I115" s="41"/>
-    </row>
-    <row r="116" spans="1:243" ht="25" customHeight="1">
-      <c r="A116" s="29"/>
-      <c r="B116" s="30"/>
-      <c r="C116" s="30"/>
-      <c r="D116" s="30"/>
-      <c r="E116" s="41"/>
-      <c r="F116" s="42"/>
-      <c r="G116" s="43"/>
-      <c r="H116" s="41"/>
-      <c r="I116" s="41"/>
-    </row>
-    <row r="117" spans="1:243" ht="20">
-      <c r="B117" s="5"/>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="33" t="s">
+      <c r="M118" s="27"/>
+    </row>
+    <row r="119" spans="1:243" ht="25" customHeight="1">
+      <c r="A119" s="29"/>
+      <c r="B119" s="30"/>
+      <c r="C119" s="30"/>
+      <c r="D119" s="30"/>
+      <c r="E119" s="41"/>
+      <c r="F119" s="42"/>
+      <c r="G119" s="43"/>
+      <c r="H119" s="41"/>
+      <c r="I119" s="41"/>
+    </row>
+    <row r="120" spans="1:243" ht="25" customHeight="1">
+      <c r="A120" s="29"/>
+      <c r="B120" s="30"/>
+      <c r="C120" s="30"/>
+      <c r="D120" s="30"/>
+      <c r="E120" s="41"/>
+      <c r="F120" s="42"/>
+      <c r="G120" s="43"/>
+      <c r="H120" s="41"/>
+      <c r="I120" s="41"/>
+    </row>
+    <row r="121" spans="1:243" ht="25" customHeight="1">
+      <c r="A121" s="29"/>
+      <c r="B121" s="30"/>
+      <c r="C121" s="30"/>
+      <c r="D121" s="30"/>
+      <c r="E121" s="41"/>
+      <c r="F121" s="42"/>
+      <c r="G121" s="43"/>
+      <c r="H121" s="41"/>
+      <c r="I121" s="41"/>
+    </row>
+    <row r="122" spans="1:243" ht="20">
+      <c r="B122" s="5"/>
+      <c r="C122" s="5"/>
+      <c r="D122" s="5"/>
+      <c r="E122" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="F117" s="35"/>
-      <c r="G117" s="44"/>
-      <c r="H117" s="38"/>
-      <c r="I117" s="38"/>
-      <c r="J117" s="15">
-        <f>SUM(J3:J112)/COUNTIF(J3:J112,"&lt;&gt;0")</f>
+      <c r="F122" s="35"/>
+      <c r="G122" s="44"/>
+      <c r="H122" s="38"/>
+      <c r="I122" s="38"/>
+      <c r="J122" s="15">
+        <f>SUM(J3:J117)/COUNTIF(J3:J117,"&lt;&gt;0")</f>
         <v>0.16565938791030202</v>
       </c>
-      <c r="K117" s="5"/>
-      <c r="L117" s="5"/>
-    </row>
-    <row r="118" spans="1:243" ht="42">
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="45" t="s">
+      <c r="K122" s="5"/>
+      <c r="L122" s="5"/>
+    </row>
+    <row r="123" spans="1:243" ht="42">
+      <c r="B123" s="5"/>
+      <c r="C123" s="5"/>
+      <c r="D123" s="5"/>
+      <c r="E123" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="F118" s="46"/>
-      <c r="G118" s="36"/>
-      <c r="H118" s="38"/>
-      <c r="I118" s="38"/>
-      <c r="J118" s="12"/>
-      <c r="K118" s="12"/>
-      <c r="L118" s="12"/>
-    </row>
-    <row r="119" spans="1:243" ht="25" customHeight="1">
-      <c r="B119" s="12"/>
-      <c r="C119" s="12"/>
-      <c r="D119" s="12"/>
-      <c r="E119" s="45" t="s">
+      <c r="F123" s="46"/>
+      <c r="G123" s="36"/>
+      <c r="H123" s="38"/>
+      <c r="I123" s="38"/>
+      <c r="J123" s="12"/>
+      <c r="K123" s="12"/>
+      <c r="L123" s="12"/>
+    </row>
+    <row r="124" spans="1:243" ht="25" customHeight="1">
+      <c r="B124" s="12"/>
+      <c r="C124" s="12"/>
+      <c r="D124" s="12"/>
+      <c r="E124" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="F119" s="46">
-        <f>COUNTIF(F3:F113, "&gt;0")</f>
-        <v>78</v>
-      </c>
-      <c r="G119" s="45"/>
-      <c r="H119" s="38"/>
-      <c r="I119" s="38"/>
-      <c r="J119" s="5"/>
-      <c r="K119" s="5"/>
-      <c r="L119" s="5"/>
-      <c r="IE119" s="7"/>
-      <c r="IF119" s="7"/>
-      <c r="IG119" s="7"/>
-      <c r="IH119" s="7"/>
-      <c r="II119" s="7"/>
-    </row>
-    <row r="120" spans="1:243" ht="25" customHeight="1">
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="33" t="s">
-        <v>117</v>
-      </c>
-      <c r="F120" s="35">
-        <v>160.13</v>
-      </c>
-      <c r="G120" s="44"/>
-      <c r="H120" s="38"/>
-      <c r="I120" s="38"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="5"/>
-      <c r="L120" s="5"/>
-      <c r="IE120" s="7"/>
-      <c r="IF120" s="7"/>
-      <c r="IG120" s="7"/>
-      <c r="IH120" s="7"/>
-      <c r="II120" s="7"/>
-    </row>
-    <row r="121" spans="1:243" ht="25" customHeight="1">
-      <c r="B121" s="5"/>
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="33" t="s">
-        <v>118</v>
-      </c>
-      <c r="F121" s="35" t="s">
-        <v>14</v>
-      </c>
-      <c r="G121" s="44"/>
-      <c r="H121" s="38"/>
-      <c r="I121" s="38"/>
-      <c r="J121" s="4"/>
-      <c r="K121" s="4"/>
-      <c r="L121" s="4"/>
-      <c r="IE121" s="7"/>
-      <c r="IF121" s="7"/>
-      <c r="IG121" s="7"/>
-      <c r="IH121" s="7"/>
-      <c r="II121" s="7"/>
-    </row>
-    <row r="122" spans="1:243" ht="25" customHeight="1">
-      <c r="B122" s="4"/>
-      <c r="C122" s="4"/>
-      <c r="D122" s="4"/>
-      <c r="E122" s="33" t="s">
-        <v>121</v>
-      </c>
-      <c r="F122" s="35">
-        <v>30</v>
-      </c>
-      <c r="G122" s="41"/>
-      <c r="H122" s="33"/>
-      <c r="I122" s="33"/>
-      <c r="J122" s="4"/>
-      <c r="K122" s="4"/>
-      <c r="L122" s="4"/>
-      <c r="IE122" s="7"/>
-      <c r="IF122" s="7"/>
-      <c r="IG122" s="7"/>
-      <c r="IH122" s="7"/>
-      <c r="II122" s="7"/>
-    </row>
-    <row r="123" spans="1:243" ht="25" customHeight="1">
-      <c r="B123" s="4"/>
-      <c r="C123" s="4"/>
-      <c r="D123" s="4"/>
-      <c r="E123" s="33" t="s">
-        <v>122</v>
-      </c>
-      <c r="F123" s="35">
-        <v>10</v>
-      </c>
-      <c r="G123" s="33"/>
-      <c r="H123" s="33"/>
-      <c r="I123" s="33"/>
-      <c r="J123" s="4"/>
-      <c r="K123" s="4"/>
-      <c r="L123" s="4"/>
-      <c r="IE123" s="7"/>
-      <c r="IF123" s="7"/>
-      <c r="IG123" s="7"/>
-      <c r="IH123" s="7"/>
-      <c r="II123" s="7"/>
-    </row>
-    <row r="124" spans="1:243" ht="25" customHeight="1">
-      <c r="B124" s="4"/>
-      <c r="C124" s="4"/>
-      <c r="D124" s="4"/>
-      <c r="E124" s="33" t="s">
-        <v>123</v>
-      </c>
-      <c r="F124" s="35" t="s">
-        <v>124</v>
-      </c>
-      <c r="G124" s="33"/>
-      <c r="H124" s="33"/>
-      <c r="I124" s="33"/>
-      <c r="J124" s="4"/>
-      <c r="K124" s="4"/>
-      <c r="L124" s="4"/>
+      <c r="F124" s="46">
+        <f>COUNTIF(F3:F118, "&gt;0")</f>
+        <v>82</v>
+      </c>
+      <c r="G124" s="45"/>
+      <c r="H124" s="38"/>
+      <c r="I124" s="38"/>
+      <c r="J124" s="5"/>
+      <c r="K124" s="5"/>
+      <c r="L124" s="5"/>
       <c r="IE124" s="7"/>
       <c r="IF124" s="7"/>
       <c r="IG124" s="7"/>
@@ -9711,16 +9873,21 @@
       <c r="II124" s="7"/>
     </row>
     <row r="125" spans="1:243" ht="25" customHeight="1">
-      <c r="B125" s="4"/>
-      <c r="C125" s="4"/>
-      <c r="D125" s="2"/>
-      <c r="E125" s="33"/>
-      <c r="F125" s="35"/>
-      <c r="G125" s="33"/>
-      <c r="H125" s="33"/>
-      <c r="I125" s="33"/>
-      <c r="K125" s="9"/>
-      <c r="L125" s="6"/>
+      <c r="B125" s="5"/>
+      <c r="C125" s="5"/>
+      <c r="D125" s="5"/>
+      <c r="E125" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="F125" s="35">
+        <v>160.13</v>
+      </c>
+      <c r="G125" s="44"/>
+      <c r="H125" s="38"/>
+      <c r="I125" s="38"/>
+      <c r="J125" s="5"/>
+      <c r="K125" s="5"/>
+      <c r="L125" s="5"/>
       <c r="IE125" s="7"/>
       <c r="IF125" s="7"/>
       <c r="IG125" s="7"/>
@@ -9728,11 +9895,21 @@
       <c r="II125" s="7"/>
     </row>
     <row r="126" spans="1:243" ht="25" customHeight="1">
-      <c r="E126" s="33"/>
-      <c r="F126" s="35"/>
-      <c r="G126" s="33"/>
-      <c r="K126" s="9"/>
-      <c r="L126" s="6"/>
+      <c r="B126" s="5"/>
+      <c r="C126" s="5"/>
+      <c r="D126" s="5"/>
+      <c r="E126" s="33" t="s">
+        <v>118</v>
+      </c>
+      <c r="F126" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="G126" s="44"/>
+      <c r="H126" s="38"/>
+      <c r="I126" s="38"/>
+      <c r="J126" s="4"/>
+      <c r="K126" s="4"/>
+      <c r="L126" s="4"/>
       <c r="IE126" s="7"/>
       <c r="IF126" s="7"/>
       <c r="IG126" s="7"/>
@@ -9740,8 +9917,21 @@
       <c r="II126" s="7"/>
     </row>
     <row r="127" spans="1:243" ht="25" customHeight="1">
-      <c r="K127" s="9"/>
-      <c r="L127" s="6"/>
+      <c r="B127" s="4"/>
+      <c r="C127" s="4"/>
+      <c r="D127" s="4"/>
+      <c r="E127" s="33" t="s">
+        <v>121</v>
+      </c>
+      <c r="F127" s="35">
+        <v>30</v>
+      </c>
+      <c r="G127" s="41"/>
+      <c r="H127" s="33"/>
+      <c r="I127" s="33"/>
+      <c r="J127" s="4"/>
+      <c r="K127" s="4"/>
+      <c r="L127" s="4"/>
       <c r="IE127" s="7"/>
       <c r="IF127" s="7"/>
       <c r="IG127" s="7"/>
@@ -9749,8 +9939,21 @@
       <c r="II127" s="7"/>
     </row>
     <row r="128" spans="1:243" ht="25" customHeight="1">
-      <c r="K128" s="9"/>
-      <c r="L128" s="6"/>
+      <c r="B128" s="4"/>
+      <c r="C128" s="4"/>
+      <c r="D128" s="4"/>
+      <c r="E128" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F128" s="35">
+        <v>10</v>
+      </c>
+      <c r="G128" s="33"/>
+      <c r="H128" s="33"/>
+      <c r="I128" s="33"/>
+      <c r="J128" s="4"/>
+      <c r="K128" s="4"/>
+      <c r="L128" s="4"/>
       <c r="IE128" s="7"/>
       <c r="IF128" s="7"/>
       <c r="IG128" s="7"/>
@@ -9758,8 +9961,21 @@
       <c r="II128" s="7"/>
     </row>
     <row r="129" spans="2:243" ht="25" customHeight="1">
-      <c r="K129" s="9"/>
-      <c r="L129" s="6"/>
+      <c r="B129" s="4"/>
+      <c r="C129" s="4"/>
+      <c r="D129" s="4"/>
+      <c r="E129" s="33" t="s">
+        <v>123</v>
+      </c>
+      <c r="F129" s="35" t="s">
+        <v>124</v>
+      </c>
+      <c r="G129" s="33"/>
+      <c r="H129" s="33"/>
+      <c r="I129" s="33"/>
+      <c r="J129" s="4"/>
+      <c r="K129" s="4"/>
+      <c r="L129" s="4"/>
       <c r="IE129" s="7"/>
       <c r="IF129" s="7"/>
       <c r="IG129" s="7"/>
@@ -9767,6 +9983,14 @@
       <c r="II129" s="7"/>
     </row>
     <row r="130" spans="2:243" ht="25" customHeight="1">
+      <c r="B130" s="4"/>
+      <c r="C130" s="4"/>
+      <c r="D130" s="2"/>
+      <c r="E130" s="33"/>
+      <c r="F130" s="35"/>
+      <c r="G130" s="33"/>
+      <c r="H130" s="33"/>
+      <c r="I130" s="33"/>
       <c r="K130" s="9"/>
       <c r="L130" s="6"/>
       <c r="IE130" s="7"/>
@@ -9776,15 +10000,9 @@
       <c r="II130" s="7"/>
     </row>
     <row r="131" spans="2:243" ht="25" customHeight="1">
-      <c r="B131" s="7"/>
-      <c r="C131" s="7"/>
-      <c r="D131" s="7"/>
-      <c r="E131" s="51"/>
-      <c r="F131" s="51"/>
-      <c r="G131" s="51"/>
-      <c r="H131" s="51"/>
-      <c r="I131" s="51"/>
-      <c r="J131" s="7"/>
+      <c r="E131" s="33"/>
+      <c r="F131" s="35"/>
+      <c r="G131" s="33"/>
       <c r="K131" s="9"/>
       <c r="L131" s="6"/>
       <c r="IE131" s="7"/>
@@ -9794,15 +10012,6 @@
       <c r="II131" s="7"/>
     </row>
     <row r="132" spans="2:243" ht="25" customHeight="1">
-      <c r="B132" s="7"/>
-      <c r="C132" s="7"/>
-      <c r="D132" s="7"/>
-      <c r="E132" s="51"/>
-      <c r="F132" s="51"/>
-      <c r="G132" s="51"/>
-      <c r="H132" s="51"/>
-      <c r="I132" s="51"/>
-      <c r="J132" s="7"/>
       <c r="K132" s="9"/>
       <c r="L132" s="6"/>
       <c r="IE132" s="7"/>
@@ -9812,15 +10021,6 @@
       <c r="II132" s="7"/>
     </row>
     <row r="133" spans="2:243" ht="25" customHeight="1">
-      <c r="B133" s="7"/>
-      <c r="C133" s="7"/>
-      <c r="D133" s="7"/>
-      <c r="E133" s="51"/>
-      <c r="F133" s="51"/>
-      <c r="G133" s="51"/>
-      <c r="H133" s="51"/>
-      <c r="I133" s="51"/>
-      <c r="J133" s="7"/>
       <c r="K133" s="9"/>
       <c r="L133" s="6"/>
       <c r="IE133" s="7"/>
@@ -9830,15 +10030,6 @@
       <c r="II133" s="7"/>
     </row>
     <row r="134" spans="2:243" ht="25" customHeight="1">
-      <c r="B134" s="7"/>
-      <c r="C134" s="7"/>
-      <c r="D134" s="7"/>
-      <c r="E134" s="51"/>
-      <c r="F134" s="51"/>
-      <c r="G134" s="51"/>
-      <c r="H134" s="51"/>
-      <c r="I134" s="51"/>
-      <c r="J134" s="7"/>
       <c r="K134" s="9"/>
       <c r="L134" s="6"/>
       <c r="IE134" s="7"/>
@@ -9847,12 +10038,98 @@
       <c r="IH134" s="7"/>
       <c r="II134" s="7"/>
     </row>
+    <row r="135" spans="2:243" ht="25" customHeight="1">
+      <c r="K135" s="9"/>
+      <c r="L135" s="6"/>
+      <c r="IE135" s="7"/>
+      <c r="IF135" s="7"/>
+      <c r="IG135" s="7"/>
+      <c r="IH135" s="7"/>
+      <c r="II135" s="7"/>
+    </row>
+    <row r="136" spans="2:243" ht="25" customHeight="1">
+      <c r="B136" s="7"/>
+      <c r="C136" s="7"/>
+      <c r="D136" s="7"/>
+      <c r="E136" s="51"/>
+      <c r="F136" s="51"/>
+      <c r="G136" s="51"/>
+      <c r="H136" s="51"/>
+      <c r="I136" s="51"/>
+      <c r="J136" s="7"/>
+      <c r="K136" s="9"/>
+      <c r="L136" s="6"/>
+      <c r="IE136" s="7"/>
+      <c r="IF136" s="7"/>
+      <c r="IG136" s="7"/>
+      <c r="IH136" s="7"/>
+      <c r="II136" s="7"/>
+    </row>
+    <row r="137" spans="2:243" ht="25" customHeight="1">
+      <c r="B137" s="7"/>
+      <c r="C137" s="7"/>
+      <c r="D137" s="7"/>
+      <c r="E137" s="51"/>
+      <c r="F137" s="51"/>
+      <c r="G137" s="51"/>
+      <c r="H137" s="51"/>
+      <c r="I137" s="51"/>
+      <c r="J137" s="7"/>
+      <c r="K137" s="9"/>
+      <c r="L137" s="6"/>
+      <c r="IE137" s="7"/>
+      <c r="IF137" s="7"/>
+      <c r="IG137" s="7"/>
+      <c r="IH137" s="7"/>
+      <c r="II137" s="7"/>
+    </row>
+    <row r="138" spans="2:243" ht="25" customHeight="1">
+      <c r="B138" s="7"/>
+      <c r="C138" s="7"/>
+      <c r="D138" s="7"/>
+      <c r="E138" s="51"/>
+      <c r="F138" s="51"/>
+      <c r="G138" s="51"/>
+      <c r="H138" s="51"/>
+      <c r="I138" s="51"/>
+      <c r="J138" s="7"/>
+      <c r="K138" s="9"/>
+      <c r="L138" s="6"/>
+      <c r="IE138" s="7"/>
+      <c r="IF138" s="7"/>
+      <c r="IG138" s="7"/>
+      <c r="IH138" s="7"/>
+      <c r="II138" s="7"/>
+    </row>
+    <row r="139" spans="2:243" ht="25" customHeight="1">
+      <c r="B139" s="7"/>
+      <c r="C139" s="7"/>
+      <c r="D139" s="7"/>
+      <c r="E139" s="51"/>
+      <c r="F139" s="51"/>
+      <c r="G139" s="51"/>
+      <c r="H139" s="51"/>
+      <c r="I139" s="51"/>
+      <c r="J139" s="7"/>
+      <c r="K139" s="9"/>
+      <c r="L139" s="6"/>
+      <c r="IE139" s="7"/>
+      <c r="IF139" s="7"/>
+      <c r="IG139" s="7"/>
+      <c r="IH139" s="7"/>
+      <c r="II139" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B115:D115"/>
+    <mergeCell ref="B116:D116"/>
+    <mergeCell ref="B117:D117"/>
+    <mergeCell ref="B118:D118"/>
     <mergeCell ref="B110:D110"/>
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B112:D112"/>
     <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B114:D114"/>
     <mergeCell ref="B105:D105"/>
     <mergeCell ref="B106:D106"/>
     <mergeCell ref="B107:D107"/>
@@ -9893,16 +10170,11 @@
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
     <mergeCell ref="E1:H1"/>
     <mergeCell ref="I1:K1"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
Upload homework-03-final-grade.xlsx, update homework-01-final-grade.xlsx and homework-02-final-grade.xlsx
</commit_message>
<xml_diff>
--- a/Supplements/homework-01-final-grade.xlsx
+++ b/Supplements/homework-01-final-grade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/研究生课程/多核程序设计与实践（助教）/homework-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF63797-4C1B-E14E-B5BE-9D323EDD04AC}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C985794-22E9-8E4A-AD2C-DF0D76540689}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="178">
   <si>
     <t>实验报告</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -572,13 +572,7 @@
     <t>OpenMP源文件编译失败</t>
   </si>
   <si>
-    <t>Makefile中未包含CUDA编译指令，且CUDA源文件使用了多文件</t>
-  </si>
-  <si>
     <t>输出的性能评测影响了结果评测程序</t>
-  </si>
-  <si>
-    <t>OpenMP源文件编译失败,CUDA输出结果错误</t>
   </si>
   <si>
     <t>OpenMP程序编译错误</t>
@@ -752,10 +746,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>程序运行出现段错误</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>提交的作业命名有问题，需要手动修改名称后才能正常运行</t>
   </si>
   <si>
@@ -802,10 +792,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>CUDA程序和OpenMP程序都编译失败</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>结果全0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -820,6 +806,58 @@
   <si>
     <t>扣5分复查分</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA编译失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>BCB3394FD061765DF70A2DF028DA4846</t>
+  </si>
+  <si>
+    <t>复查扣5分</t>
+  </si>
+  <si>
+    <r>
+      <t>复查扣</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="16"/>
+        <color indexed="8"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>分</t>
+    </r>
+  </si>
+  <si>
+    <t>08E341365F1EC38623460434A89FE2B7</t>
+  </si>
+  <si>
+    <t>OpenMP输出错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA测试性能无反应；OMP编译未通过,复查扣5分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CUDA测试性能无反应，复查扣5分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2CB562202765E68DED86A99A7BAC9C1</t>
   </si>
 </sst>
 </file>
@@ -1006,7 +1044,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1100,14 +1138,11 @@
     <xf numFmtId="177" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1118,8 +1153,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3732,8 +3779,8 @@
   </sheetPr>
   <dimension ref="A1:II142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A87" zoomScale="82" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100:D100"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="25" customHeight="1"/>
@@ -3760,22 +3807,22 @@
       <c r="A1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="31" t="s">
+      <c r="B1" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
       <c r="L1" s="3" t="s">
         <v>6</v>
       </c>
@@ -3983,7 +4030,7 @@
         <v>89</v>
       </c>
       <c r="M6" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="25" customHeight="1">
@@ -4229,7 +4276,7 @@
         <v>96</v>
       </c>
       <c r="M12" s="12" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="25" customHeight="1">
@@ -4352,7 +4399,7 @@
         <v>95</v>
       </c>
       <c r="M15" s="13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="25" customHeight="1">
@@ -4719,7 +4766,7 @@
         <v>71</v>
       </c>
       <c r="M24" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="25" spans="1:13" ht="25" customHeight="1">
@@ -5127,7 +5174,7 @@
         <v>72</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="35" spans="1:243" ht="25" customHeight="1">
@@ -5454,7 +5501,7 @@
         <v>86.932040816326534</v>
       </c>
       <c r="M42" s="11" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:243" ht="25" customHeight="1">
@@ -5497,7 +5544,7 @@
         <v>62.576530612244895</v>
       </c>
       <c r="M43" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:243" ht="25" customHeight="1">
@@ -6351,7 +6398,7 @@
         <v>70</v>
       </c>
       <c r="M47" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:243" ht="25" customHeight="1">
@@ -6435,7 +6482,7 @@
         <v>80</v>
       </c>
       <c r="M49" s="30" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:243" ht="25" customHeight="1">
@@ -6483,7 +6530,7 @@
     </row>
     <row r="51" spans="1:243" ht="25" customHeight="1">
       <c r="A51" s="25" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B51" s="8">
         <v>8</v>
@@ -6521,7 +6568,7 @@
         <v>78.858367346938778</v>
       </c>
       <c r="M51" s="10" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="IG51" s="25"/>
       <c r="IH51" s="25"/>
@@ -6529,7 +6576,7 @@
     </row>
     <row r="52" spans="1:243" ht="25" customHeight="1">
       <c r="A52" s="25" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B52" s="8">
         <v>9</v>
@@ -6573,7 +6620,7 @@
     </row>
     <row r="53" spans="1:243" ht="25" customHeight="1">
       <c r="A53" s="25" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B53" s="8">
         <v>6</v>
@@ -6616,7 +6663,7 @@
     </row>
     <row r="54" spans="1:243" ht="25" customHeight="1">
       <c r="A54" s="25" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B54" s="8">
         <v>9</v>
@@ -6659,7 +6706,7 @@
     </row>
     <row r="55" spans="1:243" ht="25" customHeight="1">
       <c r="A55" s="25" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B55" s="8">
         <v>10</v>
@@ -6702,7 +6749,7 @@
     </row>
     <row r="56" spans="1:243" ht="25" customHeight="1">
       <c r="A56" s="25" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="B56" s="8">
         <v>8</v>
@@ -6740,7 +6787,7 @@
         <v>88.24979591836734</v>
       </c>
       <c r="M56" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="IG56" s="25"/>
       <c r="IH56" s="25"/>
@@ -6872,7 +6919,7 @@
         <v>91</v>
       </c>
       <c r="M59" s="11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="IG59" s="25"/>
       <c r="IH59" s="25"/>
@@ -6918,7 +6965,7 @@
         <v>17</v>
       </c>
       <c r="M60" s="15" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="IG60" s="25"/>
       <c r="IH60" s="25"/>
@@ -7051,7 +7098,7 @@
         <v>67.5</v>
       </c>
       <c r="M63" s="11" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="IG63" s="25"/>
       <c r="IH63" s="25"/>
@@ -7093,7 +7140,7 @@
         <v>5</v>
       </c>
       <c r="L64" s="3">
-        <f t="shared" ref="L64:L119" si="2">IF(SUM(B64:E64,G64,H64:I64,K64)&lt;100, SUM(B64:E64,G64,H64:I64,K64),  100)</f>
+        <f t="shared" ref="L64:L116" si="2">IF(SUM(B64:E64,G64,H64:I64,K64)&lt;100, SUM(B64:E64,G64,H64:I64,K64),  100)</f>
         <v>96.194775510204082</v>
       </c>
       <c r="IG64" s="25"/>
@@ -7104,11 +7151,11 @@
       <c r="A65" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="B65" s="32">
+      <c r="B65" s="36">
         <v>27</v>
       </c>
-      <c r="C65" s="32"/>
-      <c r="D65" s="32"/>
+      <c r="C65" s="36"/>
+      <c r="D65" s="36"/>
       <c r="E65" s="14">
         <v>30</v>
       </c>
@@ -7144,11 +7191,11 @@
       <c r="A66" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B66" s="32">
-        <v>30</v>
-      </c>
-      <c r="C66" s="32"/>
-      <c r="D66" s="32"/>
+      <c r="B66" s="36">
+        <v>30</v>
+      </c>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
       <c r="E66" s="14">
         <v>30</v>
       </c>
@@ -7183,11 +7230,11 @@
       <c r="A67" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B67" s="32">
-        <v>30</v>
-      </c>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32"/>
+      <c r="B67" s="36">
+        <v>30</v>
+      </c>
+      <c r="C67" s="36"/>
+      <c r="D67" s="36"/>
       <c r="E67" s="14">
         <v>30</v>
       </c>
@@ -7225,11 +7272,11 @@
       <c r="A68" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="B68" s="32">
+      <c r="B68" s="36">
         <v>24</v>
       </c>
-      <c r="C68" s="32"/>
-      <c r="D68" s="32"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="36"/>
       <c r="E68" s="14">
         <v>30</v>
       </c>
@@ -7267,13 +7314,13 @@
       <c r="A69" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="B69" s="32">
+      <c r="B69" s="36">
         <v>24</v>
       </c>
-      <c r="C69" s="32"/>
-      <c r="D69" s="32"/>
+      <c r="C69" s="36"/>
+      <c r="D69" s="36"/>
       <c r="E69" s="14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F69" s="16">
         <v>0</v>
@@ -7295,11 +7342,10 @@
         <v>2.5</v>
       </c>
       <c r="L69" s="3">
-        <f t="shared" si="2"/>
-        <v>29</v>
-      </c>
-      <c r="M69" s="11" t="s">
-        <v>134</v>
+        <v>54</v>
+      </c>
+      <c r="M69" s="15" t="s">
+        <v>175</v>
       </c>
       <c r="IG69" s="25"/>
       <c r="IH69" s="25"/>
@@ -7309,11 +7355,11 @@
       <c r="A70" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="34">
+      <c r="B70" s="33">
         <v>24</v>
       </c>
-      <c r="C70" s="35"/>
-      <c r="D70" s="36"/>
+      <c r="C70" s="34"/>
+      <c r="D70" s="35"/>
       <c r="E70" s="4">
         <v>29.644970414201186</v>
       </c>
@@ -7348,11 +7394,11 @@
       <c r="A71" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B71" s="34">
+      <c r="B71" s="33">
         <v>21</v>
       </c>
-      <c r="C71" s="34"/>
-      <c r="D71" s="34"/>
+      <c r="C71" s="33"/>
+      <c r="D71" s="33"/>
       <c r="E71" s="4">
         <v>0</v>
       </c>
@@ -7380,7 +7426,7 @@
         <v>27</v>
       </c>
       <c r="M71" s="30" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="IG71" s="25"/>
       <c r="IH71" s="25"/>
@@ -7390,11 +7436,11 @@
       <c r="A72" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="B72" s="32">
+      <c r="B72" s="36">
         <v>24</v>
       </c>
-      <c r="C72" s="32"/>
-      <c r="D72" s="32"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
       <c r="E72" s="14">
         <v>30</v>
       </c>
@@ -7432,11 +7478,11 @@
       <c r="A73" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="B73" s="32">
+      <c r="B73" s="36">
         <v>27</v>
       </c>
-      <c r="C73" s="32"/>
-      <c r="D73" s="32"/>
+      <c r="C73" s="36"/>
+      <c r="D73" s="36"/>
       <c r="E73" s="14">
         <v>30</v>
       </c>
@@ -7474,11 +7520,11 @@
       <c r="A74" s="25" t="s">
         <v>80</v>
       </c>
-      <c r="B74" s="32">
+      <c r="B74" s="36">
         <v>24</v>
       </c>
-      <c r="C74" s="32"/>
-      <c r="D74" s="32"/>
+      <c r="C74" s="36"/>
+      <c r="D74" s="36"/>
       <c r="E74" s="14">
         <v>30</v>
       </c>
@@ -7516,11 +7562,11 @@
       <c r="A75" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="B75" s="32">
+      <c r="B75" s="36">
         <v>21</v>
       </c>
-      <c r="C75" s="32"/>
-      <c r="D75" s="32"/>
+      <c r="C75" s="36"/>
+      <c r="D75" s="36"/>
       <c r="E75" s="4">
         <v>30</v>
       </c>
@@ -7547,7 +7593,7 @@
         <v>91</v>
       </c>
       <c r="M75" s="30" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="IG75" s="25"/>
       <c r="IH75" s="25"/>
@@ -7557,11 +7603,11 @@
       <c r="A76" s="25" t="s">
         <v>82</v>
       </c>
-      <c r="B76" s="32">
-        <v>30</v>
-      </c>
-      <c r="C76" s="32"/>
-      <c r="D76" s="32"/>
+      <c r="B76" s="36">
+        <v>30</v>
+      </c>
+      <c r="C76" s="36"/>
+      <c r="D76" s="36"/>
       <c r="E76" s="14">
         <v>30</v>
       </c>
@@ -7596,11 +7642,11 @@
       <c r="A77" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="B77" s="32">
+      <c r="B77" s="36">
         <v>27</v>
       </c>
-      <c r="C77" s="32"/>
-      <c r="D77" s="32"/>
+      <c r="C77" s="36"/>
+      <c r="D77" s="36"/>
       <c r="E77" s="14">
         <v>0</v>
       </c>
@@ -7636,11 +7682,11 @@
       <c r="A78" s="25" t="s">
         <v>84</v>
       </c>
-      <c r="B78" s="32">
-        <v>30</v>
-      </c>
-      <c r="C78" s="32"/>
-      <c r="D78" s="32"/>
+      <c r="B78" s="36">
+        <v>30</v>
+      </c>
+      <c r="C78" s="36"/>
+      <c r="D78" s="36"/>
       <c r="E78" s="14">
         <v>30</v>
       </c>
@@ -7675,11 +7721,11 @@
       <c r="A79" s="25" t="s">
         <v>85</v>
       </c>
-      <c r="B79" s="32">
+      <c r="B79" s="36">
         <v>24</v>
       </c>
-      <c r="C79" s="32"/>
-      <c r="D79" s="32"/>
+      <c r="C79" s="36"/>
+      <c r="D79" s="36"/>
       <c r="E79" s="14">
         <v>30</v>
       </c>
@@ -7715,11 +7761,11 @@
       <c r="A80" s="25" t="s">
         <v>86</v>
       </c>
-      <c r="B80" s="32">
+      <c r="B80" s="36">
         <v>24</v>
       </c>
-      <c r="C80" s="32"/>
-      <c r="D80" s="32"/>
+      <c r="C80" s="36"/>
+      <c r="D80" s="36"/>
       <c r="E80" s="14">
         <v>30</v>
       </c>
@@ -7754,11 +7800,11 @@
       <c r="A81" s="25" t="s">
         <v>87</v>
       </c>
-      <c r="B81" s="32">
+      <c r="B81" s="36">
         <v>27</v>
       </c>
-      <c r="C81" s="32"/>
-      <c r="D81" s="32"/>
+      <c r="C81" s="36"/>
+      <c r="D81" s="36"/>
       <c r="E81" s="14">
         <v>30</v>
       </c>
@@ -7794,11 +7840,11 @@
       <c r="A82" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="B82" s="32">
+      <c r="B82" s="36">
         <v>21</v>
       </c>
-      <c r="C82" s="32"/>
-      <c r="D82" s="32"/>
+      <c r="C82" s="36"/>
+      <c r="D82" s="36"/>
       <c r="E82" s="14">
         <v>0</v>
       </c>
@@ -7836,11 +7882,11 @@
       <c r="A83" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="B83" s="32">
+      <c r="B83" s="36">
         <v>24</v>
       </c>
-      <c r="C83" s="32"/>
-      <c r="D83" s="32"/>
+      <c r="C83" s="36"/>
+      <c r="D83" s="36"/>
       <c r="E83" s="14">
         <v>30</v>
       </c>
@@ -7875,11 +7921,11 @@
       <c r="A84" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="B84" s="32">
+      <c r="B84" s="36">
         <v>24</v>
       </c>
-      <c r="C84" s="32"/>
-      <c r="D84" s="32"/>
+      <c r="C84" s="36"/>
+      <c r="D84" s="36"/>
       <c r="E84" s="4">
         <v>30</v>
       </c>
@@ -7915,11 +7961,11 @@
       <c r="A85" s="25" t="s">
         <v>89</v>
       </c>
-      <c r="B85" s="32">
+      <c r="B85" s="36">
         <v>21</v>
       </c>
-      <c r="C85" s="32"/>
-      <c r="D85" s="32"/>
+      <c r="C85" s="36"/>
+      <c r="D85" s="36"/>
       <c r="E85" s="14">
         <v>30</v>
       </c>
@@ -7955,11 +8001,11 @@
       <c r="A86" s="25" t="s">
         <v>90</v>
       </c>
-      <c r="B86" s="32">
+      <c r="B86" s="36">
         <v>24</v>
       </c>
-      <c r="C86" s="32"/>
-      <c r="D86" s="32"/>
+      <c r="C86" s="36"/>
+      <c r="D86" s="36"/>
       <c r="E86" s="14">
         <v>30</v>
       </c>
@@ -7994,11 +8040,11 @@
       <c r="A87" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="B87" s="32">
-        <v>30</v>
-      </c>
-      <c r="C87" s="32"/>
-      <c r="D87" s="32"/>
+      <c r="B87" s="36">
+        <v>30</v>
+      </c>
+      <c r="C87" s="36"/>
+      <c r="D87" s="36"/>
       <c r="E87" s="14">
         <v>30</v>
       </c>
@@ -8034,11 +8080,11 @@
       <c r="A88" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="B88" s="32">
+      <c r="B88" s="36">
         <v>24</v>
       </c>
-      <c r="C88" s="32"/>
-      <c r="D88" s="32"/>
+      <c r="C88" s="36"/>
+      <c r="D88" s="36"/>
       <c r="E88" s="14">
         <v>30</v>
       </c>
@@ -8073,11 +8119,11 @@
       <c r="A89" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="B89" s="32">
+      <c r="B89" s="36">
         <v>27</v>
       </c>
-      <c r="C89" s="32"/>
-      <c r="D89" s="32"/>
+      <c r="C89" s="36"/>
+      <c r="D89" s="36"/>
       <c r="E89" s="14">
         <v>30</v>
       </c>
@@ -8113,11 +8159,11 @@
       <c r="A90" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B90" s="34">
+      <c r="B90" s="33">
         <v>21</v>
       </c>
-      <c r="C90" s="34"/>
-      <c r="D90" s="34"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
       <c r="E90" s="4">
         <v>30</v>
       </c>
@@ -8153,11 +8199,11 @@
       <c r="A91" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B91" s="32">
+      <c r="B91" s="36">
         <v>27</v>
       </c>
-      <c r="C91" s="32"/>
-      <c r="D91" s="32"/>
+      <c r="C91" s="36"/>
+      <c r="D91" s="36"/>
       <c r="E91" s="4">
         <v>0</v>
       </c>
@@ -8184,8 +8230,8 @@
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="M91" s="37" t="s">
-        <v>171</v>
+      <c r="M91" s="32" t="s">
+        <v>167</v>
       </c>
       <c r="IG91" s="25"/>
       <c r="IH91" s="25"/>
@@ -8195,11 +8241,11 @@
       <c r="A92" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B92" s="32">
-        <v>30</v>
-      </c>
-      <c r="C92" s="32"/>
-      <c r="D92" s="32"/>
+      <c r="B92" s="36">
+        <v>30</v>
+      </c>
+      <c r="C92" s="36"/>
+      <c r="D92" s="36"/>
       <c r="E92" s="14">
         <v>30</v>
       </c>
@@ -8234,13 +8280,13 @@
       <c r="A93" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="B93" s="32">
+      <c r="B93" s="36">
         <v>21</v>
       </c>
-      <c r="C93" s="32"/>
-      <c r="D93" s="32"/>
+      <c r="C93" s="36"/>
+      <c r="D93" s="36"/>
       <c r="E93" s="14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F93" s="16">
         <v>0</v>
@@ -8262,11 +8308,10 @@
         <v>2.5</v>
       </c>
       <c r="L93" s="3">
-        <f t="shared" si="2"/>
-        <v>36</v>
-      </c>
-      <c r="M93" s="11" t="s">
-        <v>138</v>
+        <v>61</v>
+      </c>
+      <c r="M93" s="40" t="s">
+        <v>176</v>
       </c>
       <c r="IG93" s="25"/>
       <c r="IH93" s="25"/>
@@ -8276,11 +8321,11 @@
       <c r="A94" s="25" t="s">
         <v>96</v>
       </c>
-      <c r="B94" s="32">
-        <v>0</v>
-      </c>
-      <c r="C94" s="32"/>
-      <c r="D94" s="32"/>
+      <c r="B94" s="36">
+        <v>0</v>
+      </c>
+      <c r="C94" s="36"/>
+      <c r="D94" s="36"/>
       <c r="E94" s="14">
         <v>0</v>
       </c>
@@ -8318,11 +8363,11 @@
       <c r="A95" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B95" s="32">
+      <c r="B95" s="36">
         <v>27</v>
       </c>
-      <c r="C95" s="32"/>
-      <c r="D95" s="32"/>
+      <c r="C95" s="36"/>
+      <c r="D95" s="36"/>
       <c r="E95" s="14">
         <v>30</v>
       </c>
@@ -8358,11 +8403,11 @@
       <c r="A96" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="B96" s="32">
+      <c r="B96" s="36">
         <v>21</v>
       </c>
-      <c r="C96" s="32"/>
-      <c r="D96" s="32"/>
+      <c r="C96" s="36"/>
+      <c r="D96" s="36"/>
       <c r="E96" s="14">
         <v>30</v>
       </c>
@@ -8397,11 +8442,11 @@
       <c r="A97" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="B97" s="32">
+      <c r="B97" s="36">
         <v>24</v>
       </c>
-      <c r="C97" s="32"/>
-      <c r="D97" s="32"/>
+      <c r="C97" s="36"/>
+      <c r="D97" s="36"/>
       <c r="E97" s="14">
         <v>30</v>
       </c>
@@ -8437,11 +8482,11 @@
       <c r="A98" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B98" s="32">
-        <v>30</v>
-      </c>
-      <c r="C98" s="32"/>
-      <c r="D98" s="32"/>
+      <c r="B98" s="36">
+        <v>30</v>
+      </c>
+      <c r="C98" s="36"/>
+      <c r="D98" s="36"/>
       <c r="E98" s="14">
         <v>30</v>
       </c>
@@ -8476,11 +8521,11 @@
       <c r="A99" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="B99" s="32">
-        <v>30</v>
-      </c>
-      <c r="C99" s="32"/>
-      <c r="D99" s="32"/>
+      <c r="B99" s="36">
+        <v>30</v>
+      </c>
+      <c r="C99" s="36"/>
+      <c r="D99" s="36"/>
       <c r="E99" s="14">
         <v>30</v>
       </c>
@@ -8513,11 +8558,11 @@
       <c r="A100" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B100" s="32">
+      <c r="B100" s="36">
         <v>21</v>
       </c>
-      <c r="C100" s="32"/>
-      <c r="D100" s="32"/>
+      <c r="C100" s="36"/>
+      <c r="D100" s="36"/>
       <c r="E100" s="14">
         <v>30</v>
       </c>
@@ -8549,11 +8594,11 @@
       <c r="A101" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="B101" s="32">
+      <c r="B101" s="36">
         <v>21</v>
       </c>
-      <c r="C101" s="32"/>
-      <c r="D101" s="32"/>
+      <c r="C101" s="36"/>
+      <c r="D101" s="36"/>
       <c r="E101" s="14">
         <v>17.751479289940828</v>
       </c>
@@ -8586,11 +8631,11 @@
       <c r="A102" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B102" s="32">
+      <c r="B102" s="36">
         <v>21</v>
       </c>
-      <c r="C102" s="32"/>
-      <c r="D102" s="32"/>
+      <c r="C102" s="36"/>
+      <c r="D102" s="36"/>
       <c r="E102" s="14">
         <v>29.822485207100591</v>
       </c>
@@ -8618,18 +8663,18 @@
         <v>80.707791329549565</v>
       </c>
       <c r="M102" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="103" spans="1:243" ht="25" customHeight="1">
       <c r="A103" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="B103" s="32">
+      <c r="B103" s="36">
         <v>24</v>
       </c>
-      <c r="C103" s="32"/>
-      <c r="D103" s="32"/>
+      <c r="C103" s="36"/>
+      <c r="D103" s="36"/>
       <c r="E103" s="14">
         <v>30</v>
       </c>
@@ -8662,11 +8707,11 @@
       <c r="A104" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B104" s="32">
+      <c r="B104" s="36">
         <v>27</v>
       </c>
-      <c r="C104" s="32"/>
-      <c r="D104" s="32"/>
+      <c r="C104" s="36"/>
+      <c r="D104" s="36"/>
       <c r="E104" s="14">
         <v>30</v>
       </c>
@@ -8701,26 +8746,26 @@
       <c r="A105" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="32">
+      <c r="B105" s="36">
         <v>24</v>
       </c>
-      <c r="C105" s="32"/>
-      <c r="D105" s="32"/>
+      <c r="C105" s="36"/>
+      <c r="D105" s="36"/>
       <c r="E105" s="14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F105" s="16">
-        <v>0</v>
+        <v>7.3570000000000002</v>
       </c>
       <c r="G105" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.906734693877553</v>
       </c>
       <c r="H105" s="14">
         <v>2.5</v>
       </c>
       <c r="I105" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J105" s="2">
         <v>1.952367</v>
@@ -8729,22 +8774,21 @@
         <v>4.5</v>
       </c>
       <c r="L105" s="3">
-        <f t="shared" si="2"/>
-        <v>31</v>
-      </c>
-      <c r="M105" s="11" t="s">
-        <v>140</v>
+        <v>94</v>
+      </c>
+      <c r="M105" s="30" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="106" spans="1:243" ht="25" customHeight="1">
       <c r="A106" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B106" s="32">
+      <c r="B106" s="36">
         <v>27</v>
       </c>
-      <c r="C106" s="32"/>
-      <c r="D106" s="32"/>
+      <c r="C106" s="36"/>
+      <c r="D106" s="36"/>
       <c r="E106" s="14">
         <v>30</v>
       </c>
@@ -8776,11 +8820,11 @@
       <c r="A107" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="B107" s="32">
-        <v>30</v>
-      </c>
-      <c r="C107" s="32"/>
-      <c r="D107" s="32"/>
+      <c r="B107" s="36">
+        <v>30</v>
+      </c>
+      <c r="C107" s="36"/>
+      <c r="D107" s="36"/>
       <c r="E107" s="14">
         <v>30</v>
       </c>
@@ -8813,11 +8857,11 @@
       <c r="A108" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="B108" s="32">
+      <c r="B108" s="36">
         <v>21</v>
       </c>
-      <c r="C108" s="32"/>
-      <c r="D108" s="32"/>
+      <c r="C108" s="36"/>
+      <c r="D108" s="36"/>
       <c r="E108" s="14">
         <v>30</v>
       </c>
@@ -8849,11 +8893,11 @@
       <c r="A109" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="B109" s="32">
+      <c r="B109" s="36">
         <v>24</v>
       </c>
-      <c r="C109" s="32"/>
-      <c r="D109" s="32"/>
+      <c r="C109" s="36"/>
+      <c r="D109" s="36"/>
       <c r="E109" s="14">
         <v>0</v>
       </c>
@@ -8881,18 +8925,18 @@
         <v>38</v>
       </c>
       <c r="M109" s="11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="110" spans="1:243" ht="25" customHeight="1">
       <c r="A110" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="B110" s="32">
+      <c r="B110" s="36">
         <v>15</v>
       </c>
-      <c r="C110" s="32"/>
-      <c r="D110" s="32"/>
+      <c r="C110" s="36"/>
+      <c r="D110" s="36"/>
       <c r="E110" s="14">
         <v>0</v>
       </c>
@@ -8920,27 +8964,27 @@
         <v>21</v>
       </c>
       <c r="M110" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="111" spans="1:243" ht="25" customHeight="1">
       <c r="A111" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="B111" s="32">
+      <c r="B111" s="36">
         <v>21</v>
       </c>
-      <c r="C111" s="32"/>
-      <c r="D111" s="32"/>
+      <c r="C111" s="36"/>
+      <c r="D111" s="36"/>
       <c r="E111" s="14">
         <v>30</v>
       </c>
       <c r="F111" s="16">
-        <v>0</v>
+        <v>14.209</v>
       </c>
       <c r="G111" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>27.508367346938776</v>
       </c>
       <c r="H111" s="14">
         <v>5</v>
@@ -8955,22 +8999,21 @@
         <v>2.2928994082840237</v>
       </c>
       <c r="L111" s="3">
-        <f t="shared" si="2"/>
-        <v>68.292899408284029</v>
-      </c>
-      <c r="M111" s="11" t="s">
-        <v>152</v>
+        <v>90</v>
+      </c>
+      <c r="M111" s="30" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="112" spans="1:243" ht="25" customHeight="1">
       <c r="A112" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="B112" s="32">
+      <c r="B112" s="36">
         <v>21</v>
       </c>
-      <c r="C112" s="32"/>
-      <c r="D112" s="32"/>
+      <c r="C112" s="36"/>
+      <c r="D112" s="36"/>
       <c r="E112" s="14">
         <v>30</v>
       </c>
@@ -9002,11 +9045,11 @@
       <c r="A113" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="B113" s="32">
+      <c r="B113" s="36">
         <v>27</v>
       </c>
-      <c r="C113" s="32"/>
-      <c r="D113" s="32"/>
+      <c r="C113" s="36"/>
+      <c r="D113" s="36"/>
       <c r="E113" s="14">
         <v>29.644970414201186</v>
       </c>
@@ -9037,7 +9080,7 @@
     </row>
     <row r="114" spans="1:243" ht="25" customHeight="1">
       <c r="A114" s="25" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="B114" s="24">
         <v>6</v>
@@ -9055,7 +9098,7 @@
         <v>5.843</v>
       </c>
       <c r="G114" s="29">
-        <f t="shared" ref="G114:G119" si="4">IF(F114&gt;0, IF(F114&lt;2, 30, IF(F114&gt;100, 10, (1-(F114-2)/(100-2))*20+10)), 0)</f>
+        <f t="shared" ref="G114:G122" si="4">IF(F114&gt;0, IF(F114&lt;2, 30, IF(F114&gt;100, 10, (1-(F114-2)/(100-2))*20+10)), 0)</f>
         <v>29.215714285714284</v>
       </c>
       <c r="H114" s="4">
@@ -9075,12 +9118,12 @@
         <v>82.860684699915467</v>
       </c>
       <c r="M114" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="115" spans="1:243" s="27" customFormat="1" ht="25" customHeight="1">
       <c r="A115" s="27" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="B115" s="26">
         <v>10</v>
@@ -9351,7 +9394,7 @@
     </row>
     <row r="116" spans="1:243" ht="25" customHeight="1">
       <c r="A116" s="25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B116" s="24">
         <v>6</v>
@@ -9392,7 +9435,7 @@
     </row>
     <row r="117" spans="1:243" ht="25" customHeight="1">
       <c r="A117" s="25" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B117" s="24">
         <v>6</v>
@@ -9404,20 +9447,20 @@
         <v>6</v>
       </c>
       <c r="E117" s="4">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F117" s="2">
-        <v>0</v>
+        <v>1.8776999999999999</v>
       </c>
       <c r="G117" s="29">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H117" s="4">
         <v>3</v>
       </c>
       <c r="I117" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J117" s="2">
         <v>0</v>
@@ -9426,16 +9469,15 @@
         <v>3</v>
       </c>
       <c r="L117" s="3">
-        <f t="shared" si="2"/>
-        <v>24</v>
+        <v>89</v>
       </c>
       <c r="M117" s="30" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="118" spans="1:243" ht="25" customHeight="1">
       <c r="A118" s="25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="B118" s="24">
         <v>6</v>
@@ -9469,14 +9511,14 @@
         <v>3</v>
       </c>
       <c r="L118" s="3">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(B118:E118,G118,H118:I118,K118)&lt;100, SUM(B118:E118,G118,H118:I118,K118),  100)</f>
         <v>93.200909189711382</v>
       </c>
       <c r="M118" s="11"/>
     </row>
     <row r="119" spans="1:243" ht="25" customHeight="1">
       <c r="A119" s="25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B119" s="24">
         <v>6</v>
@@ -9510,7 +9552,7 @@
         <v>3</v>
       </c>
       <c r="L119" s="3">
-        <f t="shared" si="2"/>
+        <f>IF(SUM(B119:E119,G119,H119:I119,K119)&lt;100, SUM(B119:E119,G119,H119:I119,K119),  100)</f>
         <v>93.644970414201183</v>
       </c>
       <c r="M119" s="30"/>
@@ -9521,8 +9563,47 @@
       <c r="II119" s="25"/>
     </row>
     <row r="120" spans="1:243" ht="25" customHeight="1">
-      <c r="G120" s="19"/>
-      <c r="H120" s="14"/>
+      <c r="A120" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="B120" s="31">
+        <v>6</v>
+      </c>
+      <c r="C120" s="24">
+        <v>6</v>
+      </c>
+      <c r="D120" s="24">
+        <v>0</v>
+      </c>
+      <c r="E120" s="14">
+        <v>0</v>
+      </c>
+      <c r="F120" s="16">
+        <v>0</v>
+      </c>
+      <c r="G120" s="29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H120" s="14">
+        <v>4</v>
+      </c>
+      <c r="I120" s="14">
+        <v>10</v>
+      </c>
+      <c r="J120" s="2">
+        <v>0</v>
+      </c>
+      <c r="K120" s="4">
+        <v>4</v>
+      </c>
+      <c r="L120" s="3">
+        <f>IF(SUM(B120:E120,G120,H120:I120,K120)&lt;100, SUM(B120:E120,G120,H120:I120,K120),  100)</f>
+        <v>30</v>
+      </c>
+      <c r="M120" s="39" t="s">
+        <v>169</v>
+      </c>
       <c r="IE120" s="25"/>
       <c r="IF120" s="25"/>
       <c r="IG120" s="25"/>
@@ -9530,8 +9611,44 @@
       <c r="II120" s="25"/>
     </row>
     <row r="121" spans="1:243" ht="25" customHeight="1">
-      <c r="G121" s="19"/>
-      <c r="H121" s="14"/>
+      <c r="A121" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="B121" s="24">
+        <v>6</v>
+      </c>
+      <c r="C121" s="24">
+        <v>6</v>
+      </c>
+      <c r="D121" s="24">
+        <v>8</v>
+      </c>
+      <c r="E121" s="14">
+        <v>30</v>
+      </c>
+      <c r="F121" s="16">
+        <v>0.83099999999999996</v>
+      </c>
+      <c r="G121" s="29">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H121" s="14">
+        <v>4</v>
+      </c>
+      <c r="I121" s="14">
+        <v>10</v>
+      </c>
+      <c r="J121" s="2">
+        <v>0</v>
+      </c>
+      <c r="K121" s="4">
+        <v>4</v>
+      </c>
+      <c r="L121" s="3">
+        <f>IF(SUM(B121:E121,G121,H121:I121,K121)&lt;100, SUM(B121:E121,G121,H121:I121,K121),  100)</f>
+        <v>98</v>
+      </c>
       <c r="IE121" s="25"/>
       <c r="IF121" s="25"/>
       <c r="IG121" s="25"/>
@@ -9539,8 +9656,44 @@
       <c r="II121" s="25"/>
     </row>
     <row r="122" spans="1:243" ht="25" customHeight="1">
-      <c r="G122" s="19"/>
-      <c r="H122" s="14"/>
+      <c r="A122" s="25" t="s">
+        <v>177</v>
+      </c>
+      <c r="B122" s="24">
+        <v>6</v>
+      </c>
+      <c r="C122" s="24">
+        <v>6</v>
+      </c>
+      <c r="D122" s="24">
+        <v>5</v>
+      </c>
+      <c r="E122" s="14">
+        <v>30</v>
+      </c>
+      <c r="F122" s="16">
+        <v>1.8859999999999999</v>
+      </c>
+      <c r="G122" s="29">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="H122" s="14">
+        <v>4</v>
+      </c>
+      <c r="I122" s="14">
+        <v>10</v>
+      </c>
+      <c r="J122" s="2">
+        <v>0</v>
+      </c>
+      <c r="K122" s="4">
+        <v>4</v>
+      </c>
+      <c r="L122" s="3">
+        <f>IF(SUM(B122:E122,G122,H122:I122,K122)&lt;100, SUM(B122:E122,G122,H122:I122,K122),  100)</f>
+        <v>95</v>
+      </c>
       <c r="IE122" s="25"/>
       <c r="IF122" s="25"/>
       <c r="IG122" s="25"/>
@@ -9604,7 +9757,7 @@
       </c>
       <c r="F127" s="22">
         <f>COUNTIF(F3:F113, "&gt;0")</f>
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="G127" s="21"/>
       <c r="I127" s="23"/>
@@ -9793,6 +9946,44 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B87:D87"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B109:D109"/>
     <mergeCell ref="B90:D90"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B70:D70"/>
@@ -9807,44 +9998,6 @@
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B87:D87"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>

<commit_message>
upload final-project-final-grad.xlsx and mid-term-grade.xlsx. update homework grade.
</commit_message>
<xml_diff>
--- a/Supplements/homework-01-final-grade.xlsx
+++ b/Supplements/homework-01-final-grade.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/william/Documents/研究生课程/多核程序设计与实践（助教）/homework-01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C985794-22E9-8E4A-AD2C-DF0D76540689}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3830C679-2F60-9F41-92FE-185D4F0FDDB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,17 @@
     <sheet name="Sheet 1 - res" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1 - res'!$L$1</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1 - res'!$L$2:$L$142</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1 - res'!$F$2</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1 - res'!$F$3:$F$113</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">'Sheet 1 - res'!$F$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'Sheet 1 - res'!$F$3:$F$113</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'Sheet 1 - res'!$L$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'Sheet 1 - res'!$L$2:$L$142</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="179">
   <si>
     <t>实验报告</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -858,6 +858,10 @@
   </si>
   <si>
     <t>C2CB562202765E68DED86A99A7BAC9C1</t>
+  </si>
+  <si>
+    <t>复查扣5分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1144,6 +1148,21 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1152,21 +1171,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1259,7 +1263,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.3</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1351,7 +1355,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{1030102B-0947-CA47-9ED9-857AE3CBF761}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.2</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>时间（ms）</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1380,7 +1384,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.1</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1426,7 +1430,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{782EC41C-AD7D-E542-8EB7-0E8059F39A56}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.0</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>总分</cx:v>
             </cx:txData>
           </cx:tx>
@@ -3779,8 +3783,8 @@
   </sheetPr>
   <dimension ref="A1:II142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="82" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A104" zoomScale="82" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="25" customHeight="1"/>
@@ -3807,17 +3811,17 @@
       <c r="A1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="37" t="s">
+      <c r="B1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="36" t="s">
         <v>1</v>
       </c>
@@ -7355,11 +7359,11 @@
       <c r="A70" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="B70" s="33">
+      <c r="B70" s="38">
         <v>24</v>
       </c>
-      <c r="C70" s="34"/>
-      <c r="D70" s="35"/>
+      <c r="C70" s="39"/>
+      <c r="D70" s="40"/>
       <c r="E70" s="4">
         <v>29.644970414201186</v>
       </c>
@@ -7394,11 +7398,11 @@
       <c r="A71" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="B71" s="33">
+      <c r="B71" s="38">
         <v>21</v>
       </c>
-      <c r="C71" s="33"/>
-      <c r="D71" s="33"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="38"/>
       <c r="E71" s="4">
         <v>0</v>
       </c>
@@ -7648,20 +7652,20 @@
       <c r="C77" s="36"/>
       <c r="D77" s="36"/>
       <c r="E77" s="14">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F77" s="16">
-        <v>0</v>
+        <v>10.811999999999999</v>
       </c>
       <c r="G77" s="19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>28.201632653061225</v>
       </c>
       <c r="H77" s="14">
         <v>2.5</v>
       </c>
       <c r="I77" s="14">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J77" s="2">
         <v>0.25622400000000001</v>
@@ -7670,10 +7674,11 @@
         <v>4.5</v>
       </c>
       <c r="L77" s="3">
-        <f t="shared" si="2"/>
-        <v>34</v>
-      </c>
-      <c r="M77" s="11"/>
+        <v>95</v>
+      </c>
+      <c r="M77" s="11" t="s">
+        <v>178</v>
+      </c>
       <c r="IG77" s="25"/>
       <c r="IH77" s="25"/>
       <c r="II77" s="25"/>
@@ -8159,11 +8164,11 @@
       <c r="A90" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="B90" s="33">
+      <c r="B90" s="38">
         <v>21</v>
       </c>
-      <c r="C90" s="33"/>
-      <c r="D90" s="33"/>
+      <c r="C90" s="38"/>
+      <c r="D90" s="38"/>
       <c r="E90" s="4">
         <v>30</v>
       </c>
@@ -8310,7 +8315,7 @@
       <c r="L93" s="3">
         <v>61</v>
       </c>
-      <c r="M93" s="40" t="s">
+      <c r="M93" s="34" t="s">
         <v>176</v>
       </c>
       <c r="IG93" s="25"/>
@@ -9601,7 +9606,7 @@
         <f>IF(SUM(B120:E120,G120,H120:I120,K120)&lt;100, SUM(B120:E120,G120,H120:I120,K120),  100)</f>
         <v>30</v>
       </c>
-      <c r="M120" s="39" t="s">
+      <c r="M120" s="33" t="s">
         <v>169</v>
       </c>
       <c r="IE120" s="25"/>
@@ -9757,7 +9762,7 @@
       </c>
       <c r="F127" s="22">
         <f>COUNTIF(F3:F113, "&gt;0")</f>
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="G127" s="21"/>
       <c r="I127" s="23"/>
@@ -9946,16 +9951,33 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="E1:H1"/>
-    <mergeCell ref="I1:K1"/>
-    <mergeCell ref="B1:D1"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B111:D111"/>
+    <mergeCell ref="B112:D112"/>
+    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="B99:D99"/>
     <mergeCell ref="B91:D91"/>
     <mergeCell ref="B92:D92"/>
     <mergeCell ref="B93:D93"/>
@@ -9965,39 +9987,22 @@
     <mergeCell ref="B87:D87"/>
     <mergeCell ref="B88:D88"/>
     <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B111:D111"/>
-    <mergeCell ref="B112:D112"/>
-    <mergeCell ref="B113:D113"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B109:D109"/>
     <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B69:D69"/>
     <mergeCell ref="B71:D71"/>
     <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="B81:D81"/>
     <mergeCell ref="B72:D72"/>
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="B74:D74"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:K1"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>

</xml_diff>